<commit_message>
Summary updated. Tasks fixed when users transpass collisions!
</commit_message>
<xml_diff>
--- a/Formated/SummaryPerCheckpoint.xlsx
+++ b/Formated/SummaryPerCheckpoint.xlsx
@@ -227,8 +227,8 @@
   </sheetPr>
   <dimension ref="A1:Z142"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A102" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A145" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -352,7 +352,7 @@
         <v>20.0589999999997</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>3</v>
       </c>
@@ -369,10 +369,10 @@
         <v>32.1591000000001</v>
       </c>
       <c r="F13" s="0" t="n">
-        <v>2.888704</v>
+        <v>4.957484</v>
       </c>
       <c r="G13" s="0" t="n">
-        <v>18.3759</v>
+        <v>19.6083</v>
       </c>
       <c r="H13" s="0" t="n">
         <v>2.416622</v>
@@ -381,7 +381,7 @@
         <v>14.7269999999999</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <v>3</v>
       </c>
@@ -401,7 +401,7 @@
         <v>2.442658</v>
       </c>
       <c r="G14" s="0" t="n">
-        <v>59.079</v>
+        <v>10.9740999999999</v>
       </c>
       <c r="H14" s="0" t="n">
         <v>2.383837</v>
@@ -410,7 +410,7 @@
         <v>16.627</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <v>3</v>
       </c>
@@ -427,10 +427,10 @@
         <v>14.2048</v>
       </c>
       <c r="F15" s="0" t="n">
-        <v>4.272902</v>
+        <v>4.814818</v>
       </c>
       <c r="G15" s="0" t="n">
-        <v>-44.7620999999999</v>
+        <v>4.81850000000009</v>
       </c>
       <c r="H15" s="0" t="n">
         <v>1.325592</v>
@@ -439,7 +439,7 @@
         <v>57.7730000000001</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
         <v>3</v>
       </c>
@@ -459,7 +459,7 @@
         <v>3.414459</v>
       </c>
       <c r="G16" s="0" t="n">
-        <v>75.8877</v>
+        <v>26.3071</v>
       </c>
       <c r="H16" s="0" t="n">
         <v>1.385773</v>
@@ -468,7 +468,7 @@
         <v>41.2539999999999</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <v>3</v>
       </c>
@@ -497,7 +497,7 @@
         <v>15.3830000000003</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
         <v>3</v>
       </c>
@@ -526,7 +526,7 @@
         <v>1.35999999999967</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
         <v>3</v>
       </c>
@@ -555,7 +555,7 @@
         <v>2.35000000000036</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
         <v>3</v>
       </c>
@@ -1059,7 +1059,7 @@
         <v>0.6788346</v>
       </c>
       <c r="I40" s="0" t="n">
-        <v>23.9505</v>
+        <v>11.5012</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1351,10 +1351,10 @@
         <v>3</v>
       </c>
       <c r="B51" s="0" t="n">
-        <v>2.803829</v>
+        <v>4.213804</v>
       </c>
       <c r="C51" s="0" t="n">
-        <v>40.3312999999999</v>
+        <v>33.33</v>
       </c>
       <c r="D51" s="0" t="n">
         <v>4.348501</v>
@@ -1380,10 +1380,10 @@
         <v>3</v>
       </c>
       <c r="B52" s="0" t="n">
-        <v>5.918599</v>
+        <v>6.246723</v>
       </c>
       <c r="C52" s="0" t="n">
-        <v>15.5892</v>
+        <v>13.2841999999999</v>
       </c>
       <c r="D52" s="0" t="n">
         <v>5.607391</v>
@@ -1412,7 +1412,7 @@
         <v>4.969846</v>
       </c>
       <c r="C53" s="0" t="n">
-        <v>100.4908</v>
+        <v>19.6085</v>
       </c>
       <c r="D53" s="0" t="n">
         <v>2.965274</v>
@@ -1438,10 +1438,10 @@
         <v>3</v>
       </c>
       <c r="B54" s="0" t="n">
-        <v>4.722402</v>
+        <v>5.75478</v>
       </c>
       <c r="C54" s="0" t="n">
-        <v>-72.3471000000001</v>
+        <v>16.2627</v>
       </c>
       <c r="D54" s="0" t="n">
         <v>4.973049</v>
@@ -1470,7 +1470,7 @@
         <v>5.762327</v>
       </c>
       <c r="C55" s="0" t="n">
-        <v>115.9088</v>
+        <v>27.299</v>
       </c>
       <c r="D55" s="0" t="n">
         <v>3.587233</v>
@@ -1586,7 +1586,7 @@
         <v>5.138432</v>
       </c>
       <c r="C59" s="0" t="n">
-        <v>59.812</v>
+        <v>9.32300000000009</v>
       </c>
       <c r="D59" s="0" t="n">
         <v>7.236197</v>
@@ -1598,7 +1598,7 @@
         <v>4.724011</v>
       </c>
       <c r="G59" s="0" t="n">
-        <v>104.0704</v>
+        <v>29.3548</v>
       </c>
       <c r="H59" s="0" t="n">
         <v>0.8447551</v>
@@ -1612,10 +1612,10 @@
         <v>4</v>
       </c>
       <c r="B60" s="0" t="n">
-        <v>3.513048</v>
+        <v>3.737296</v>
       </c>
       <c r="C60" s="0" t="n">
-        <v>-26.6199999999999</v>
+        <v>9.17000000000007</v>
       </c>
       <c r="D60" s="0" t="n">
         <v>4.201269</v>
@@ -1641,10 +1641,10 @@
         <v>4</v>
       </c>
       <c r="B61" s="0" t="n">
-        <v>5.950465</v>
+        <v>6.744919</v>
       </c>
       <c r="C61" s="0" t="n">
-        <v>6.02499999999986</v>
+        <v>21.4349999999999</v>
       </c>
       <c r="D61" s="0" t="n">
         <v>3.644014</v>
@@ -1673,7 +1673,7 @@
         <v>2.334157</v>
       </c>
       <c r="C62" s="0" t="n">
-        <v>58.5710000000001</v>
+        <v>7.37100000000009</v>
       </c>
       <c r="D62" s="0" t="n">
         <v>3.947317</v>
@@ -1682,10 +1682,10 @@
         <v>22.35446</v>
       </c>
       <c r="F62" s="0" t="n">
-        <v>2.820436</v>
+        <v>5.678527</v>
       </c>
       <c r="G62" s="0" t="n">
-        <v>-78.5279</v>
+        <v>7.5163</v>
       </c>
       <c r="H62" s="0" t="n">
         <v>1.972835</v>
@@ -1714,7 +1714,7 @@
         <v>3.985703</v>
       </c>
       <c r="G63" s="0" t="n">
-        <v>94.6022</v>
+        <v>8.55799999999999</v>
       </c>
       <c r="H63" s="0" t="n">
         <v>1.700862</v>
@@ -1917,7 +1917,7 @@
         <v>4.317525</v>
       </c>
       <c r="G70" s="0" t="n">
-        <v>87.7889</v>
+        <v>30.1441</v>
       </c>
       <c r="H70" s="0" t="n">
         <v>1.041057</v>
@@ -1943,10 +1943,10 @@
         <v>10.0856</v>
       </c>
       <c r="F71" s="0" t="n">
-        <v>2.347379</v>
+        <v>3.683563</v>
       </c>
       <c r="G71" s="0" t="n">
-        <v>-51.7610999999999</v>
+        <v>10.1146</v>
       </c>
       <c r="H71" s="0" t="n">
         <v>2.634937</v>
@@ -1975,7 +1975,7 @@
         <v>4.911202</v>
       </c>
       <c r="G72" s="0" t="n">
-        <v>70.9461</v>
+        <v>9.07040000000006</v>
       </c>
       <c r="H72" s="0" t="n">
         <v>5.505518</v>
@@ -2059,10 +2059,10 @@
         <v>6.30349999999999</v>
       </c>
       <c r="F75" s="0" t="n">
-        <v>4.408616</v>
+        <v>5.38718</v>
       </c>
       <c r="G75" s="0" t="n">
-        <v>-77.4665</v>
+        <v>1.00049999999999</v>
       </c>
       <c r="H75" s="0" t="n">
         <v>2.054172</v>
@@ -2091,7 +2091,7 @@
         <v>4.531362</v>
       </c>
       <c r="G76" s="0" t="n">
-        <v>78.6675</v>
+        <v>0.200500000000034</v>
       </c>
       <c r="H76" s="0" t="n">
         <v>1.97392</v>
@@ -2435,10 +2435,10 @@
         <v>3</v>
       </c>
       <c r="B89" s="0" t="n">
-        <v>3.697272</v>
+        <v>10.34307</v>
       </c>
       <c r="C89" s="0" t="n">
-        <v>17.4450999999999</v>
+        <v>28.7244999999999</v>
       </c>
       <c r="D89" s="0" t="n">
         <v>6.976802</v>
@@ -2461,7 +2461,7 @@
         <v>6.275187</v>
       </c>
       <c r="C90" s="0" t="n">
-        <v>117.2078</v>
+        <v>21.0163</v>
       </c>
       <c r="D90" s="0" t="n">
         <v>2.859821</v>
@@ -2854,10 +2854,10 @@
         <v>3</v>
       </c>
       <c r="D108" s="0" t="n">
-        <v>3.971377</v>
+        <v>6.838632</v>
       </c>
       <c r="E108" s="0" t="n">
-        <v>35.3665999999999</v>
+        <v>18.4039</v>
       </c>
       <c r="F108" s="0" t="n">
         <v>5.685935</v>
@@ -2871,10 +2871,10 @@
         <v>3</v>
       </c>
       <c r="D109" s="0" t="n">
-        <v>3.118359</v>
+        <v>3.861755</v>
       </c>
       <c r="E109" s="0" t="n">
-        <v>13.186</v>
+        <v>17.486</v>
       </c>
       <c r="F109" s="0" t="n">
         <v>1.319708</v>
@@ -2888,10 +2888,10 @@
         <v>3</v>
       </c>
       <c r="D110" s="0" t="n">
-        <v>3.838295</v>
+        <v>5.753842</v>
       </c>
       <c r="E110" s="0" t="n">
-        <v>16.1315999999999</v>
+        <v>27.9196999999999</v>
       </c>
       <c r="F110" s="0" t="n">
         <v>1.291296</v>
@@ -2908,7 +2908,7 @@
         <v>2.178203</v>
       </c>
       <c r="E111" s="0" t="n">
-        <v>98.2145</v>
+        <v>6.47810000000004</v>
       </c>
       <c r="F111" s="0" t="n">
         <v>2.04324</v>
@@ -3460,13 +3460,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I136"/>
+  <dimension ref="A1:S157"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A88" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K135" activeCellId="0" sqref="K135"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A116" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I150" activeCellId="0" sqref="I150"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.10526315789474"/>
   </cols>
@@ -3479,22 +3479,22 @@
         <v>2.552981</v>
       </c>
       <c r="C1" s="0" t="n">
+        <v>1.923633</v>
+      </c>
+      <c r="D1" s="0" t="n">
+        <v>0.457849</v>
+      </c>
+      <c r="E1" s="0" t="n">
+        <v>1.554914</v>
+      </c>
+      <c r="F1" s="0" t="n">
         <v>43.7014</v>
       </c>
-      <c r="D1" s="0" t="n">
-        <v>1.923633</v>
-      </c>
-      <c r="E1" s="0" t="n">
+      <c r="G1" s="0" t="n">
         <v>18.9205</v>
       </c>
-      <c r="F1" s="0" t="n">
-        <v>0.457849</v>
-      </c>
-      <c r="G1" s="0" t="n">
+      <c r="H1" s="0" t="n">
         <v>53.4206</v>
-      </c>
-      <c r="H1" s="0" t="n">
-        <v>1.554914</v>
       </c>
       <c r="I1" s="0" t="n">
         <v>42.2799999999998</v>
@@ -3507,13 +3507,13 @@
       <c r="B2" s="0" t="n">
         <v>6.00778</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="D2" s="0" t="n">
+        <v>1.276835</v>
+      </c>
+      <c r="F2" s="0" t="n">
         <v>0.599699999999984</v>
       </c>
-      <c r="F2" s="0" t="n">
-        <v>1.276835</v>
-      </c>
-      <c r="G2" s="0" t="n">
+      <c r="H2" s="0" t="n">
         <v>1.29938</v>
       </c>
     </row>
@@ -3525,22 +3525,22 @@
         <v>16.95301</v>
       </c>
       <c r="C3" s="0" t="n">
+        <v>11.75348</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>3.243309</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>3.538198</v>
+      </c>
+      <c r="F3" s="0" t="n">
         <v>27.5805</v>
       </c>
-      <c r="D3" s="0" t="n">
-        <v>11.75348</v>
-      </c>
-      <c r="E3" s="0" t="n">
+      <c r="G3" s="0" t="n">
         <v>22.0545</v>
       </c>
-      <c r="F3" s="0" t="n">
-        <v>3.243309</v>
-      </c>
-      <c r="G3" s="0" t="n">
+      <c r="H3" s="0" t="n">
         <v>15.1507</v>
-      </c>
-      <c r="H3" s="0" t="n">
-        <v>3.538198</v>
       </c>
       <c r="I3" s="0" t="n">
         <v>20.0589999999997</v>
@@ -3554,22 +3554,22 @@
         <v>6.87595</v>
       </c>
       <c r="C4" s="0" t="n">
+        <v>6.2464</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>2.557314</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>2.416622</v>
+      </c>
+      <c r="F4" s="0" t="n">
         <v>12.766</v>
       </c>
-      <c r="D4" s="0" t="n">
-        <v>6.2464</v>
-      </c>
-      <c r="E4" s="0" t="n">
+      <c r="G4" s="0" t="n">
         <v>16.5443</v>
       </c>
-      <c r="F4" s="0" t="n">
-        <v>2.557314</v>
-      </c>
-      <c r="G4" s="0" t="n">
+      <c r="H4" s="0" t="n">
         <v>21.8664</v>
-      </c>
-      <c r="H4" s="0" t="n">
-        <v>2.416622</v>
       </c>
       <c r="I4" s="0" t="n">
         <v>14.7269999999999</v>
@@ -3583,22 +3583,22 @@
         <v>6.623047</v>
       </c>
       <c r="C5" s="0" t="n">
+        <v>2.100487</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>1.822733</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>2.383837</v>
+      </c>
+      <c r="F5" s="0" t="n">
         <v>9.10759999999999</v>
       </c>
-      <c r="D5" s="0" t="n">
-        <v>2.100487</v>
-      </c>
-      <c r="E5" s="0" t="n">
+      <c r="G5" s="0" t="n">
         <v>6.5702</v>
       </c>
-      <c r="F5" s="0" t="n">
-        <v>1.822733</v>
-      </c>
-      <c r="G5" s="0" t="n">
+      <c r="H5" s="0" t="n">
         <v>8.45359999999999</v>
-      </c>
-      <c r="H5" s="0" t="n">
-        <v>2.383837</v>
       </c>
       <c r="I5" s="0" t="n">
         <v>16.627</v>
@@ -3612,22 +3612,22 @@
         <v>11.89963</v>
       </c>
       <c r="C6" s="0" t="n">
+        <v>0.9704856</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>2.709819</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>1.325592</v>
+      </c>
+      <c r="F6" s="0" t="n">
         <v>7.90820000000002</v>
       </c>
-      <c r="D6" s="0" t="n">
-        <v>0.9704856</v>
-      </c>
-      <c r="E6" s="0" t="n">
+      <c r="G6" s="0" t="n">
         <v>17.8009</v>
       </c>
-      <c r="F6" s="0" t="n">
-        <v>2.709819</v>
-      </c>
-      <c r="G6" s="0" t="n">
+      <c r="H6" s="0" t="n">
         <v>26.2541</v>
-      </c>
-      <c r="H6" s="0" t="n">
-        <v>1.325592</v>
       </c>
       <c r="I6" s="0" t="n">
         <v>57.7730000000001</v>
@@ -3641,22 +3641,22 @@
         <v>8.263282</v>
       </c>
       <c r="C7" s="0" t="n">
+        <v>2.421061</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>2.292903</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>1.385773</v>
+      </c>
+      <c r="F7" s="0" t="n">
         <v>0.807299999999998</v>
       </c>
-      <c r="D7" s="0" t="n">
-        <v>2.421061</v>
-      </c>
-      <c r="E7" s="0" t="n">
+      <c r="G7" s="0" t="n">
         <v>19.1355</v>
       </c>
-      <c r="F7" s="0" t="n">
-        <v>2.292903</v>
-      </c>
-      <c r="G7" s="0" t="n">
+      <c r="H7" s="0" t="n">
         <v>21.5064</v>
-      </c>
-      <c r="H7" s="0" t="n">
-        <v>1.385773</v>
       </c>
       <c r="I7" s="0" t="n">
         <v>41.2539999999999</v>
@@ -3670,22 +3670,22 @@
         <v>7.022774</v>
       </c>
       <c r="C8" s="0" t="n">
+        <v>1.546066</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>2.942827</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>3.100229</v>
+      </c>
+      <c r="F8" s="0" t="n">
         <v>1.35449999999997</v>
       </c>
-      <c r="D8" s="0" t="n">
-        <v>1.546066</v>
-      </c>
-      <c r="E8" s="0" t="n">
+      <c r="G8" s="0" t="n">
         <v>5.123</v>
       </c>
-      <c r="F8" s="0" t="n">
-        <v>2.942827</v>
-      </c>
-      <c r="G8" s="0" t="n">
+      <c r="H8" s="0" t="n">
         <v>24.7494</v>
-      </c>
-      <c r="H8" s="0" t="n">
-        <v>3.100229</v>
       </c>
       <c r="I8" s="0" t="n">
         <v>15.3830000000003</v>
@@ -3699,22 +3699,22 @@
         <v>8.752884</v>
       </c>
       <c r="C9" s="0" t="n">
+        <v>5.472954</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>3.568282</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>2.602042</v>
+      </c>
+      <c r="F9" s="0" t="n">
         <v>9.01150000000001</v>
       </c>
-      <c r="D9" s="0" t="n">
-        <v>5.472954</v>
-      </c>
-      <c r="E9" s="0" t="n">
+      <c r="G9" s="0" t="n">
         <v>0.801</v>
       </c>
-      <c r="F9" s="0" t="n">
-        <v>3.568282</v>
-      </c>
-      <c r="G9" s="0" t="n">
+      <c r="H9" s="0" t="n">
         <v>14.8506</v>
-      </c>
-      <c r="H9" s="0" t="n">
-        <v>2.602042</v>
       </c>
       <c r="I9" s="0" t="n">
         <v>1.35999999999967</v>
@@ -3728,22 +3728,22 @@
         <v>7.459644</v>
       </c>
       <c r="C10" s="0" t="n">
+        <v>1.739387</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>2.714013</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>2.730695</v>
+      </c>
+      <c r="F10" s="0" t="n">
         <v>0.349800000000016</v>
       </c>
-      <c r="D10" s="0" t="n">
-        <v>1.739387</v>
-      </c>
-      <c r="E10" s="0" t="n">
+      <c r="G10" s="0" t="n">
         <v>6.4623</v>
       </c>
-      <c r="F10" s="0" t="n">
-        <v>2.714013</v>
-      </c>
-      <c r="G10" s="0" t="n">
+      <c r="H10" s="0" t="n">
         <v>5.25029999999998</v>
-      </c>
-      <c r="H10" s="0" t="n">
-        <v>2.730695</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>2.35000000000036</v>
@@ -3757,22 +3757,22 @@
         <v>15.66327</v>
       </c>
       <c r="C11" s="0" t="n">
+        <v>5.513764</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>5.170437</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>3.174932</v>
+      </c>
+      <c r="F11" s="0" t="n">
         <v>2.90100000000001</v>
       </c>
-      <c r="D11" s="0" t="n">
-        <v>5.513764</v>
-      </c>
-      <c r="E11" s="0" t="n">
+      <c r="G11" s="0" t="n">
         <v>13.5254</v>
       </c>
-      <c r="F11" s="0" t="n">
-        <v>5.170437</v>
-      </c>
-      <c r="G11" s="0" t="n">
+      <c r="H11" s="0" t="n">
         <v>3.09910000000002</v>
-      </c>
-      <c r="H11" s="0" t="n">
-        <v>3.174932</v>
       </c>
       <c r="I11" s="0" t="n">
         <v>8.42699999999968</v>
@@ -3786,22 +3786,22 @@
         <v>7.257324</v>
       </c>
       <c r="C12" s="0" t="n">
+        <v>6.748151</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>3.337802</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>1.641494</v>
+      </c>
+      <c r="F12" s="0" t="n">
         <v>27.4123000000001</v>
       </c>
-      <c r="D12" s="0" t="n">
-        <v>6.748151</v>
-      </c>
-      <c r="E12" s="0" t="n">
+      <c r="G12" s="0" t="n">
         <v>9.72915</v>
       </c>
-      <c r="F12" s="0" t="n">
-        <v>3.337802</v>
-      </c>
-      <c r="G12" s="0" t="n">
+      <c r="H12" s="0" t="n">
         <v>25.0997</v>
-      </c>
-      <c r="H12" s="0" t="n">
-        <v>1.641494</v>
       </c>
       <c r="I12" s="0" t="n">
         <v>43.46362</v>
@@ -3815,22 +3815,22 @@
         <v>6.539456</v>
       </c>
       <c r="C13" s="0" t="n">
+        <v>2.78187</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>2.689958</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>1.190929</v>
+      </c>
+      <c r="F13" s="0" t="n">
         <v>7.05290000000002</v>
       </c>
-      <c r="D13" s="0" t="n">
-        <v>2.78187</v>
-      </c>
-      <c r="E13" s="0" t="n">
+      <c r="G13" s="0" t="n">
         <v>7.62127</v>
       </c>
-      <c r="F13" s="0" t="n">
-        <v>2.689958</v>
-      </c>
-      <c r="G13" s="0" t="n">
+      <c r="H13" s="0" t="n">
         <v>4.75020000000001</v>
-      </c>
-      <c r="H13" s="0" t="n">
-        <v>1.190929</v>
       </c>
       <c r="I13" s="0" t="n">
         <v>8.54754999999999</v>
@@ -3844,22 +3844,22 @@
         <v>11.11605</v>
       </c>
       <c r="C14" s="0" t="n">
+        <v>1.441352</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>3.025027</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>2.314833</v>
+      </c>
+      <c r="F14" s="0" t="n">
         <v>11.2918</v>
       </c>
-      <c r="D14" s="0" t="n">
-        <v>1.441352</v>
-      </c>
-      <c r="E14" s="0" t="n">
+      <c r="G14" s="0" t="n">
         <v>43.35246</v>
       </c>
-      <c r="F14" s="0" t="n">
-        <v>3.025027</v>
-      </c>
-      <c r="G14" s="0" t="n">
+      <c r="H14" s="0" t="n">
         <v>13.4503</v>
-      </c>
-      <c r="H14" s="0" t="n">
-        <v>2.314833</v>
       </c>
       <c r="I14" s="0" t="n">
         <v>10.55221</v>
@@ -3873,22 +3873,22 @@
         <v>9.425533</v>
       </c>
       <c r="C15" s="0" t="n">
+        <v>1.506991</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>2.12221</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>1.499431</v>
+      </c>
+      <c r="F15" s="0" t="n">
         <v>1.82420000000002</v>
       </c>
-      <c r="D15" s="0" t="n">
-        <v>1.506991</v>
-      </c>
-      <c r="E15" s="0" t="n">
+      <c r="G15" s="0" t="n">
         <v>12.99745</v>
       </c>
-      <c r="F15" s="0" t="n">
-        <v>2.12221</v>
-      </c>
-      <c r="G15" s="0" t="n">
+      <c r="H15" s="0" t="n">
         <v>6.34899999999999</v>
-      </c>
-      <c r="H15" s="0" t="n">
-        <v>1.499431</v>
       </c>
       <c r="I15" s="0" t="n">
         <v>13.74972</v>
@@ -3902,22 +3902,22 @@
         <v>10.25405</v>
       </c>
       <c r="C16" s="0" t="n">
+        <v>1.804433</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>2.627921</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>1.145168</v>
+      </c>
+      <c r="F16" s="0" t="n">
         <v>2.50900000000001</v>
       </c>
-      <c r="D16" s="0" t="n">
-        <v>1.804433</v>
-      </c>
-      <c r="E16" s="0" t="n">
+      <c r="G16" s="0" t="n">
         <v>2.01632</v>
       </c>
-      <c r="F16" s="0" t="n">
-        <v>2.627921</v>
-      </c>
-      <c r="G16" s="0" t="n">
+      <c r="H16" s="0" t="n">
         <v>10.1635</v>
-      </c>
-      <c r="H16" s="0" t="n">
-        <v>1.145168</v>
       </c>
       <c r="I16" s="0" t="n">
         <v>5.45439999999999</v>
@@ -3931,22 +3931,22 @@
         <v>4.83198</v>
       </c>
       <c r="C17" s="0" t="n">
+        <v>2.926983</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>4.488725</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>2.822591</v>
+      </c>
+      <c r="F17" s="0" t="n">
         <v>0.954399999999964</v>
       </c>
-      <c r="D17" s="0" t="n">
-        <v>2.926983</v>
-      </c>
-      <c r="E17" s="0" t="n">
+      <c r="G17" s="0" t="n">
         <v>3.61093</v>
       </c>
-      <c r="F17" s="0" t="n">
-        <v>4.488725</v>
-      </c>
-      <c r="G17" s="0" t="n">
+      <c r="H17" s="0" t="n">
         <v>6.64879999999999</v>
-      </c>
-      <c r="H17" s="0" t="n">
-        <v>2.822591</v>
       </c>
       <c r="I17" s="0" t="n">
         <v>1.4002</v>
@@ -3960,22 +3960,22 @@
         <v>9.743069</v>
       </c>
       <c r="C18" s="0" t="n">
+        <v>2.753535</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>5.045763</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>2.969541</v>
+      </c>
+      <c r="F18" s="0" t="n">
         <v>0.650399999999991</v>
       </c>
-      <c r="D18" s="0" t="n">
-        <v>2.753535</v>
-      </c>
-      <c r="E18" s="0" t="n">
+      <c r="G18" s="0" t="n">
         <v>4.1506</v>
       </c>
-      <c r="F18" s="0" t="n">
-        <v>5.045763</v>
-      </c>
-      <c r="G18" s="0" t="n">
+      <c r="H18" s="0" t="n">
         <v>0.300400000000025</v>
-      </c>
-      <c r="H18" s="0" t="n">
-        <v>2.969541</v>
       </c>
       <c r="I18" s="0" t="n">
         <v>0.749899999999997</v>
@@ -3989,22 +3989,22 @@
         <v>9.071087</v>
       </c>
       <c r="C19" s="0" t="n">
+        <v>8.802749</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>6.273589</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>3.302351</v>
+      </c>
+      <c r="F19" s="0" t="n">
         <v>4.50390000000004</v>
       </c>
-      <c r="D19" s="0" t="n">
-        <v>8.802749</v>
-      </c>
-      <c r="E19" s="0" t="n">
+      <c r="G19" s="0" t="n">
         <v>6.4688</v>
       </c>
-      <c r="F19" s="0" t="n">
-        <v>6.273589</v>
-      </c>
-      <c r="G19" s="0" t="n">
+      <c r="H19" s="0" t="n">
         <v>8.19990000000001</v>
-      </c>
-      <c r="H19" s="0" t="n">
-        <v>3.302351</v>
       </c>
       <c r="I19" s="0" t="n">
         <v>2.40220000000001</v>
@@ -4018,22 +4018,22 @@
         <v>4.031909</v>
       </c>
       <c r="C20" s="0" t="n">
+        <v>3.004579</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>1.562084</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>1.622368</v>
+      </c>
+      <c r="F20" s="0" t="n">
         <v>82.4115</v>
       </c>
-      <c r="D20" s="0" t="n">
-        <v>3.004579</v>
-      </c>
-      <c r="E20" s="0" t="n">
+      <c r="G20" s="0" t="n">
         <v>11.8498</v>
       </c>
-      <c r="F20" s="0" t="n">
-        <v>1.562084</v>
-      </c>
-      <c r="G20" s="0" t="n">
+      <c r="H20" s="0" t="n">
         <v>25.1607</v>
-      </c>
-      <c r="H20" s="0" t="n">
-        <v>1.622368</v>
       </c>
       <c r="I20" s="0" t="n">
         <v>48.95116</v>
@@ -4046,17 +4046,17 @@
       <c r="B21" s="0" t="n">
         <v>3.707431</v>
       </c>
-      <c r="C21" s="0" t="n">
+      <c r="D21" s="0" t="n">
+        <v>3.156556</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>1.62389</v>
+      </c>
+      <c r="F21" s="0" t="n">
         <v>0.501300000000015</v>
       </c>
-      <c r="F21" s="0" t="n">
-        <v>3.156556</v>
-      </c>
-      <c r="G21" s="0" t="n">
+      <c r="H21" s="0" t="n">
         <v>1.3993</v>
-      </c>
-      <c r="H21" s="0" t="n">
-        <v>1.62389</v>
       </c>
       <c r="I21" s="0" t="n">
         <v>1.95099999999999</v>
@@ -4070,22 +4070,22 @@
         <v>6.642847</v>
       </c>
       <c r="C22" s="0" t="n">
+        <v>4.069859</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>4.060901</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>2.768127</v>
+      </c>
+      <c r="F22" s="0" t="n">
         <v>25.7002</v>
       </c>
-      <c r="D22" s="0" t="n">
-        <v>4.069859</v>
-      </c>
-      <c r="E22" s="0" t="n">
+      <c r="G22" s="0" t="n">
         <v>15.153</v>
       </c>
-      <c r="F22" s="0" t="n">
-        <v>4.060901</v>
-      </c>
-      <c r="G22" s="0" t="n">
+      <c r="H22" s="0" t="n">
         <v>46.8605</v>
-      </c>
-      <c r="H22" s="0" t="n">
-        <v>2.768127</v>
       </c>
       <c r="I22" s="0" t="n">
         <v>23.2197</v>
@@ -4099,22 +4099,22 @@
         <v>5.797201</v>
       </c>
       <c r="C23" s="0" t="n">
+        <v>4.348501</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>4.823443</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>0.8555403</v>
+      </c>
+      <c r="F23" s="0" t="n">
         <v>54.7911</v>
       </c>
-      <c r="D23" s="0" t="n">
-        <v>4.348501</v>
-      </c>
-      <c r="E23" s="0" t="n">
+      <c r="G23" s="0" t="n">
         <v>13.7009</v>
       </c>
-      <c r="F23" s="0" t="n">
-        <v>4.823443</v>
-      </c>
-      <c r="G23" s="0" t="n">
+      <c r="H23" s="0" t="n">
         <v>32.8003</v>
-      </c>
-      <c r="H23" s="0" t="n">
-        <v>0.8555403</v>
       </c>
       <c r="I23" s="0" t="n">
         <v>32.2997</v>
@@ -4128,22 +4128,22 @@
         <v>4.264198</v>
       </c>
       <c r="C24" s="0" t="n">
+        <v>5.607391</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>2.683038</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>2.229399</v>
+      </c>
+      <c r="F24" s="0" t="n">
         <v>24.7517</v>
       </c>
-      <c r="D24" s="0" t="n">
-        <v>5.607391</v>
-      </c>
-      <c r="E24" s="0" t="n">
+      <c r="G24" s="0" t="n">
         <v>14.8492</v>
       </c>
-      <c r="F24" s="0" t="n">
-        <v>2.683038</v>
-      </c>
-      <c r="G24" s="0" t="n">
+      <c r="H24" s="0" t="n">
         <v>40.2152</v>
-      </c>
-      <c r="H24" s="0" t="n">
-        <v>2.229399</v>
       </c>
       <c r="I24" s="0" t="n">
         <v>23.7017</v>
@@ -4157,22 +4157,22 @@
         <v>9.980396</v>
       </c>
       <c r="C25" s="0" t="n">
+        <v>2.965274</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>4.031501</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>3.561848</v>
+      </c>
+      <c r="F25" s="0" t="n">
         <v>7.51850000000002</v>
       </c>
-      <c r="D25" s="0" t="n">
-        <v>2.965274</v>
-      </c>
-      <c r="E25" s="0" t="n">
+      <c r="G25" s="0" t="n">
         <v>11.5508</v>
       </c>
-      <c r="F25" s="0" t="n">
-        <v>4.031501</v>
-      </c>
-      <c r="G25" s="0" t="n">
+      <c r="H25" s="0" t="n">
         <v>7.35069999999996</v>
-      </c>
-      <c r="H25" s="0" t="n">
-        <v>3.561848</v>
       </c>
       <c r="I25" s="0" t="n">
         <v>12.6035</v>
@@ -4186,22 +4186,22 @@
         <v>2.096157</v>
       </c>
       <c r="C26" s="0" t="n">
+        <v>4.973049</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>4.14871</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>1.873684</v>
+      </c>
+      <c r="F26" s="0" t="n">
         <v>12.3256</v>
       </c>
-      <c r="D26" s="0" t="n">
-        <v>4.973049</v>
-      </c>
-      <c r="E26" s="0" t="n">
+      <c r="G26" s="0" t="n">
         <v>17.4551</v>
       </c>
-      <c r="F26" s="0" t="n">
-        <v>4.14871</v>
-      </c>
-      <c r="G26" s="0" t="n">
+      <c r="H26" s="0" t="n">
         <v>4.95060000000001</v>
-      </c>
-      <c r="H26" s="0" t="n">
-        <v>1.873684</v>
       </c>
       <c r="I26" s="0" t="n">
         <v>18.21</v>
@@ -4215,22 +4215,22 @@
         <v>9.242344</v>
       </c>
       <c r="C27" s="0" t="n">
+        <v>3.587233</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>3.434093</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>1.998164</v>
+      </c>
+      <c r="F27" s="0" t="n">
         <v>2.50239999999997</v>
       </c>
-      <c r="D27" s="0" t="n">
-        <v>3.587233</v>
-      </c>
-      <c r="E27" s="0" t="n">
+      <c r="G27" s="0" t="n">
         <v>14.6002</v>
       </c>
-      <c r="F27" s="0" t="n">
-        <v>3.434093</v>
-      </c>
-      <c r="G27" s="0" t="n">
+      <c r="H27" s="0" t="n">
         <v>5.20069999999998</v>
-      </c>
-      <c r="H27" s="0" t="n">
-        <v>1.998164</v>
       </c>
       <c r="I27" s="0" t="n">
         <v>13.7527</v>
@@ -4244,22 +4244,22 @@
         <v>5.441056</v>
       </c>
       <c r="C28" s="0" t="n">
+        <v>4.286748</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>2.817188</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <v>0.9204666</v>
+      </c>
+      <c r="F28" s="0" t="n">
         <v>0.250599999999963</v>
       </c>
-      <c r="D28" s="0" t="n">
-        <v>4.286748</v>
-      </c>
-      <c r="E28" s="0" t="n">
+      <c r="G28" s="0" t="n">
         <v>6.75269999999995</v>
       </c>
-      <c r="F28" s="0" t="n">
-        <v>2.817188</v>
-      </c>
-      <c r="G28" s="0" t="n">
+      <c r="H28" s="0" t="n">
         <v>3.44920000000002</v>
-      </c>
-      <c r="H28" s="0" t="n">
-        <v>0.9204666</v>
       </c>
       <c r="I28" s="0" t="n">
         <v>4.90050000000002</v>
@@ -4273,22 +4273,22 @@
         <v>3.757367</v>
       </c>
       <c r="C29" s="0" t="n">
+        <v>4.492808</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>4.17964</v>
+      </c>
+      <c r="E29" s="0" t="n">
+        <v>1.17128</v>
+      </c>
+      <c r="F29" s="0" t="n">
         <v>10.8469</v>
       </c>
-      <c r="D29" s="0" t="n">
-        <v>4.492808</v>
-      </c>
-      <c r="E29" s="0" t="n">
+      <c r="G29" s="0" t="n">
         <v>2.45090000000005</v>
       </c>
-      <c r="F29" s="0" t="n">
-        <v>4.17964</v>
-      </c>
-      <c r="G29" s="0" t="n">
+      <c r="H29" s="0" t="n">
         <v>15.9521</v>
-      </c>
-      <c r="H29" s="0" t="n">
-        <v>1.17128</v>
       </c>
       <c r="I29" s="0" t="n">
         <v>3.65679999999998</v>
@@ -4302,22 +4302,22 @@
         <v>18.47361</v>
       </c>
       <c r="C30" s="0" t="n">
+        <v>8.534507</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>5.710479</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <v>1.599064</v>
+      </c>
+      <c r="F30" s="0" t="n">
         <v>14.2433</v>
       </c>
-      <c r="D30" s="0" t="n">
-        <v>8.534507</v>
-      </c>
-      <c r="E30" s="0" t="n">
+      <c r="G30" s="0" t="n">
         <v>5.25299999999999</v>
       </c>
-      <c r="F30" s="0" t="n">
-        <v>5.710479</v>
-      </c>
-      <c r="G30" s="0" t="n">
+      <c r="H30" s="0" t="n">
         <v>8.40369999999996</v>
-      </c>
-      <c r="H30" s="0" t="n">
-        <v>1.599064</v>
       </c>
       <c r="I30" s="0" t="n">
         <v>12.1</v>
@@ -4331,25 +4331,25 @@
         <v>3.160902</v>
       </c>
       <c r="C31" s="0" t="n">
+        <v>7.236197</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>4.724011</v>
+      </c>
+      <c r="E31" s="0" t="n">
+        <v>0.6788346</v>
+      </c>
+      <c r="F31" s="0" t="n">
         <v>18.7913</v>
       </c>
-      <c r="D31" s="0" t="n">
-        <v>7.236197</v>
-      </c>
-      <c r="E31" s="0" t="n">
+      <c r="G31" s="0" t="n">
         <v>16.35614</v>
       </c>
-      <c r="F31" s="0" t="n">
-        <v>4.724011</v>
-      </c>
-      <c r="G31" s="0" t="n">
-        <v>104.0704</v>
-      </c>
       <c r="H31" s="0" t="n">
-        <v>0.6788346</v>
+        <v>29.3548</v>
       </c>
       <c r="I31" s="0" t="n">
-        <v>23.9505</v>
+        <v>11.5012</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4360,22 +4360,22 @@
         <v>5.515357</v>
       </c>
       <c r="C32" s="0" t="n">
+        <v>4.201269</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>1.438804</v>
+      </c>
+      <c r="E32" s="0" t="n">
+        <v>2.35458</v>
+      </c>
+      <c r="F32" s="0" t="n">
         <v>18.4734999999999</v>
       </c>
-      <c r="D32" s="0" t="n">
-        <v>4.201269</v>
-      </c>
-      <c r="E32" s="0" t="n">
+      <c r="G32" s="0" t="n">
         <v>6.55044</v>
       </c>
-      <c r="F32" s="0" t="n">
-        <v>1.438804</v>
-      </c>
-      <c r="G32" s="0" t="n">
+      <c r="H32" s="0" t="n">
         <v>15.0597</v>
-      </c>
-      <c r="H32" s="0" t="n">
-        <v>2.35458</v>
       </c>
       <c r="I32" s="0" t="n">
         <v>10.8049</v>
@@ -4389,22 +4389,22 @@
         <v>9.930317</v>
       </c>
       <c r="C33" s="0" t="n">
+        <v>3.644014</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <v>2.808136</v>
+      </c>
+      <c r="E33" s="0" t="n">
+        <v>1.352477</v>
+      </c>
+      <c r="F33" s="0" t="n">
         <v>7.76760000000002</v>
       </c>
-      <c r="D33" s="0" t="n">
-        <v>3.644014</v>
-      </c>
-      <c r="E33" s="0" t="n">
+      <c r="G33" s="0" t="n">
         <v>14.30109</v>
       </c>
-      <c r="F33" s="0" t="n">
-        <v>2.808136</v>
-      </c>
-      <c r="G33" s="0" t="n">
+      <c r="H33" s="0" t="n">
         <v>13.6096</v>
-      </c>
-      <c r="H33" s="0" t="n">
-        <v>1.352477</v>
       </c>
       <c r="I33" s="0" t="n">
         <v>8.40660000000003</v>
@@ -4418,22 +4418,22 @@
         <v>3.052425</v>
       </c>
       <c r="C34" s="0" t="n">
+        <v>3.947317</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>5.678527</v>
+      </c>
+      <c r="E34" s="0" t="n">
+        <v>1.090702</v>
+      </c>
+      <c r="F34" s="0" t="n">
         <v>14.4149</v>
       </c>
-      <c r="D34" s="0" t="n">
-        <v>3.947317</v>
-      </c>
-      <c r="E34" s="0" t="n">
+      <c r="G34" s="0" t="n">
         <v>22.35446</v>
       </c>
-      <c r="F34" s="0" t="n">
-        <v>2.820436</v>
-      </c>
-      <c r="G34" s="0" t="n">
-        <v>-78.5279</v>
-      </c>
       <c r="H34" s="0" t="n">
-        <v>1.090702</v>
+        <v>7.5163</v>
       </c>
       <c r="I34" s="0" t="n">
         <v>2.80029999999999</v>
@@ -4447,22 +4447,22 @@
         <v>3.591951</v>
       </c>
       <c r="C35" s="0" t="n">
+        <v>2.317144</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <v>3.985703</v>
+      </c>
+      <c r="E35" s="0" t="n">
+        <v>2.379631</v>
+      </c>
+      <c r="F35" s="0" t="n">
         <v>2.9122000000001</v>
       </c>
-      <c r="D35" s="0" t="n">
-        <v>2.317144</v>
-      </c>
-      <c r="E35" s="0" t="n">
+      <c r="G35" s="0" t="n">
         <v>28.90913</v>
       </c>
-      <c r="F35" s="0" t="n">
-        <v>3.985703</v>
-      </c>
-      <c r="G35" s="0" t="n">
-        <v>94.6022</v>
-      </c>
       <c r="H35" s="0" t="n">
-        <v>2.379631</v>
+        <v>8.55799999999999</v>
       </c>
       <c r="I35" s="0" t="n">
         <v>6.00080000000003</v>
@@ -4476,22 +4476,22 @@
         <v>4.161583</v>
       </c>
       <c r="C36" s="0" t="n">
+        <v>2.617777</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <v>2.050389</v>
+      </c>
+      <c r="E36" s="0" t="n">
+        <v>3.19397</v>
+      </c>
+      <c r="F36" s="0" t="n">
         <v>11.2849</v>
       </c>
-      <c r="D36" s="0" t="n">
-        <v>2.617777</v>
-      </c>
-      <c r="E36" s="0" t="n">
+      <c r="G36" s="0" t="n">
         <v>5.84949999999999</v>
       </c>
-      <c r="F36" s="0" t="n">
-        <v>2.050389</v>
-      </c>
-      <c r="G36" s="0" t="n">
+      <c r="H36" s="0" t="n">
         <v>5.20499999999993</v>
-      </c>
-      <c r="H36" s="0" t="n">
-        <v>3.19397</v>
       </c>
       <c r="I36" s="0" t="n">
         <v>3.74919999999997</v>
@@ -4505,22 +4505,22 @@
         <v>3.437613</v>
       </c>
       <c r="C37" s="0" t="n">
+        <v>0.9864246</v>
+      </c>
+      <c r="D37" s="0" t="n">
+        <v>2.517652</v>
+      </c>
+      <c r="E37" s="0" t="n">
+        <v>3.084859</v>
+      </c>
+      <c r="F37" s="0" t="n">
         <v>7.62599999999998</v>
       </c>
-      <c r="D37" s="0" t="n">
-        <v>0.9864246</v>
-      </c>
-      <c r="E37" s="0" t="n">
+      <c r="G37" s="0" t="n">
         <v>13.6</v>
       </c>
-      <c r="F37" s="0" t="n">
-        <v>2.517652</v>
-      </c>
-      <c r="G37" s="0" t="n">
+      <c r="H37" s="0" t="n">
         <v>5.7111000000001</v>
-      </c>
-      <c r="H37" s="0" t="n">
-        <v>3.084859</v>
       </c>
       <c r="I37" s="0" t="n">
         <v>1.35040000000004</v>
@@ -4534,22 +4534,22 @@
         <v>12.79405</v>
       </c>
       <c r="C38" s="0" t="n">
+        <v>11.14828</v>
+      </c>
+      <c r="D38" s="0" t="n">
+        <v>4.083905</v>
+      </c>
+      <c r="E38" s="0" t="n">
+        <v>1.093341</v>
+      </c>
+      <c r="F38" s="0" t="n">
         <v>6.5865</v>
       </c>
-      <c r="D38" s="0" t="n">
-        <v>11.14828</v>
-      </c>
-      <c r="E38" s="0" t="n">
+      <c r="G38" s="0" t="n">
         <v>4.9503</v>
       </c>
-      <c r="F38" s="0" t="n">
-        <v>4.083905</v>
-      </c>
-      <c r="G38" s="0" t="n">
+      <c r="H38" s="0" t="n">
         <v>6.09719999999993</v>
-      </c>
-      <c r="H38" s="0" t="n">
-        <v>1.093341</v>
       </c>
       <c r="I38" s="0" t="n">
         <v>16.1541</v>
@@ -4563,22 +4563,22 @@
         <v>1.317529</v>
       </c>
       <c r="C39" s="0" t="n">
+        <v>2.033778</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <v>1.233917</v>
+      </c>
+      <c r="E39" s="0" t="n">
+        <v>1.062217</v>
+      </c>
+      <c r="F39" s="0" t="n">
         <v>32.4661</v>
       </c>
-      <c r="D39" s="0" t="n">
-        <v>2.033778</v>
-      </c>
-      <c r="E39" s="0" t="n">
+      <c r="G39" s="0" t="n">
         <v>13.4501</v>
       </c>
-      <c r="F39" s="0" t="n">
-        <v>1.233917</v>
-      </c>
-      <c r="G39" s="0" t="n">
+      <c r="H39" s="0" t="n">
         <v>32.9624</v>
-      </c>
-      <c r="H39" s="0" t="n">
-        <v>1.062217</v>
       </c>
       <c r="I39" s="0" t="n">
         <v>19.40325</v>
@@ -4592,22 +4592,22 @@
         <v>3.203304</v>
       </c>
       <c r="C40" s="0" t="n">
+        <v>2.351931</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <v>3.28459</v>
+      </c>
+      <c r="E40" s="0" t="n">
+        <v>1.742188</v>
+      </c>
+      <c r="F40" s="0" t="n">
         <v>0.749599999999987</v>
       </c>
-      <c r="D40" s="0" t="n">
-        <v>2.351931</v>
-      </c>
-      <c r="E40" s="0" t="n">
+      <c r="G40" s="0" t="n">
         <v>2.24939999999998</v>
       </c>
-      <c r="F40" s="0" t="n">
-        <v>3.28459</v>
-      </c>
-      <c r="G40" s="0" t="n">
+      <c r="H40" s="0" t="n">
         <v>1.1995</v>
-      </c>
-      <c r="H40" s="0" t="n">
-        <v>1.742188</v>
       </c>
       <c r="I40" s="0" t="n">
         <v>1.34997</v>
@@ -4621,22 +4621,22 @@
         <v>9.220284</v>
       </c>
       <c r="C41" s="0" t="n">
+        <v>5.547572</v>
+      </c>
+      <c r="D41" s="0" t="n">
+        <v>3.317118</v>
+      </c>
+      <c r="E41" s="0" t="n">
+        <v>4.50141</v>
+      </c>
+      <c r="F41" s="0" t="n">
         <v>27.9945</v>
       </c>
-      <c r="D41" s="0" t="n">
-        <v>5.547572</v>
-      </c>
-      <c r="E41" s="0" t="n">
+      <c r="G41" s="0" t="n">
         <v>12.8002</v>
       </c>
-      <c r="F41" s="0" t="n">
-        <v>3.317118</v>
-      </c>
-      <c r="G41" s="0" t="n">
+      <c r="H41" s="0" t="n">
         <v>18.8063</v>
-      </c>
-      <c r="H41" s="0" t="n">
-        <v>4.50141</v>
       </c>
       <c r="I41" s="0" t="n">
         <v>14.7503</v>
@@ -4647,25 +4647,25 @@
         <v>3</v>
       </c>
       <c r="B42" s="0" t="n">
-        <v>2.803829</v>
+        <v>4.213804</v>
       </c>
       <c r="C42" s="0" t="n">
-        <v>40.3312999999999</v>
+        <v>8.100928</v>
       </c>
       <c r="D42" s="0" t="n">
-        <v>8.100928</v>
+        <v>4.317525</v>
       </c>
       <c r="E42" s="0" t="n">
+        <v>1.669326</v>
+      </c>
+      <c r="F42" s="0" t="n">
+        <v>33.33</v>
+      </c>
+      <c r="G42" s="0" t="n">
         <v>15.7025</v>
       </c>
-      <c r="F42" s="0" t="n">
-        <v>4.317525</v>
-      </c>
-      <c r="G42" s="0" t="n">
-        <v>87.7889</v>
-      </c>
       <c r="H42" s="0" t="n">
-        <v>1.669326</v>
+        <v>30.1441</v>
       </c>
       <c r="I42" s="0" t="n">
         <v>19.8511</v>
@@ -4676,25 +4676,25 @@
         <v>3</v>
       </c>
       <c r="B43" s="0" t="n">
-        <v>5.918599</v>
+        <v>6.246723</v>
       </c>
       <c r="C43" s="0" t="n">
-        <v>15.5892</v>
+        <v>3.980249</v>
       </c>
       <c r="D43" s="0" t="n">
-        <v>3.980249</v>
+        <v>3.683563</v>
       </c>
       <c r="E43" s="0" t="n">
+        <v>2.409864</v>
+      </c>
+      <c r="F43" s="0" t="n">
+        <v>13.2841999999999</v>
+      </c>
+      <c r="G43" s="0" t="n">
         <v>10.0856</v>
       </c>
-      <c r="F43" s="0" t="n">
-        <v>2.347379</v>
-      </c>
-      <c r="G43" s="0" t="n">
-        <v>-51.7610999999999</v>
-      </c>
       <c r="H43" s="0" t="n">
-        <v>2.409864</v>
+        <v>10.1146</v>
       </c>
       <c r="I43" s="0" t="n">
         <v>18.299</v>
@@ -4708,22 +4708,22 @@
         <v>4.969846</v>
       </c>
       <c r="C44" s="0" t="n">
-        <v>100.4908</v>
+        <v>2.845469</v>
       </c>
       <c r="D44" s="0" t="n">
-        <v>2.845469</v>
+        <v>4.911202</v>
       </c>
       <c r="E44" s="0" t="n">
+        <v>3.591711</v>
+      </c>
+      <c r="F44" s="0" t="n">
+        <v>19.6085</v>
+      </c>
+      <c r="G44" s="0" t="n">
         <v>15.3092</v>
       </c>
-      <c r="F44" s="0" t="n">
-        <v>4.911202</v>
-      </c>
-      <c r="G44" s="0" t="n">
-        <v>70.9461</v>
-      </c>
       <c r="H44" s="0" t="n">
-        <v>3.591711</v>
+        <v>9.07040000000006</v>
       </c>
       <c r="I44" s="0" t="n">
         <v>11.3001</v>
@@ -4734,25 +4734,25 @@
         <v>3</v>
       </c>
       <c r="B45" s="0" t="n">
-        <v>4.722402</v>
+        <v>5.75478</v>
       </c>
       <c r="C45" s="0" t="n">
-        <v>-72.3471000000001</v>
+        <v>7.707931</v>
       </c>
       <c r="D45" s="0" t="n">
-        <v>7.707931</v>
+        <v>2.722098</v>
       </c>
       <c r="E45" s="0" t="n">
+        <v>4.685834</v>
+      </c>
+      <c r="F45" s="0" t="n">
+        <v>16.2627</v>
+      </c>
+      <c r="G45" s="0" t="n">
         <v>4.2029</v>
       </c>
-      <c r="F45" s="0" t="n">
-        <v>2.722098</v>
-      </c>
-      <c r="G45" s="0" t="n">
+      <c r="H45" s="0" t="n">
         <v>20.0798999999999</v>
-      </c>
-      <c r="H45" s="0" t="n">
-        <v>4.685834</v>
       </c>
       <c r="I45" s="0" t="n">
         <v>3.34979999999999</v>
@@ -4766,22 +4766,22 @@
         <v>5.762327</v>
       </c>
       <c r="C46" s="0" t="n">
-        <v>115.9088</v>
+        <v>4.472928</v>
       </c>
       <c r="D46" s="0" t="n">
-        <v>4.472928</v>
+        <v>3.916257</v>
       </c>
       <c r="E46" s="0" t="n">
+        <v>2.674754</v>
+      </c>
+      <c r="F46" s="0" t="n">
+        <v>27.299</v>
+      </c>
+      <c r="G46" s="0" t="n">
         <v>11.3067</v>
       </c>
-      <c r="F46" s="0" t="n">
-        <v>3.916257</v>
-      </c>
-      <c r="G46" s="0" t="n">
+      <c r="H46" s="0" t="n">
         <v>3.65589999999997</v>
-      </c>
-      <c r="H46" s="0" t="n">
-        <v>2.674754</v>
       </c>
       <c r="I46" s="0" t="n">
         <v>6.15020000000001</v>
@@ -4795,22 +4795,22 @@
         <v>7.920792</v>
       </c>
       <c r="C47" s="0" t="n">
+        <v>4.306945</v>
+      </c>
+      <c r="D47" s="0" t="n">
+        <v>5.38718</v>
+      </c>
+      <c r="E47" s="0" t="n">
+        <v>3.033717</v>
+      </c>
+      <c r="F47" s="0" t="n">
         <v>13.1084</v>
       </c>
-      <c r="D47" s="0" t="n">
-        <v>4.306945</v>
-      </c>
-      <c r="E47" s="0" t="n">
+      <c r="G47" s="0" t="n">
         <v>6.30349999999999</v>
       </c>
-      <c r="F47" s="0" t="n">
-        <v>4.408616</v>
-      </c>
-      <c r="G47" s="0" t="n">
-        <v>-77.4665</v>
-      </c>
       <c r="H47" s="0" t="n">
-        <v>3.033717</v>
+        <v>1.00049999999999</v>
       </c>
       <c r="I47" s="0" t="n">
         <v>1.90449999999998</v>
@@ -4824,22 +4824,22 @@
         <v>10.5386</v>
       </c>
       <c r="C48" s="0" t="n">
+        <v>6.1752</v>
+      </c>
+      <c r="D48" s="0" t="n">
+        <v>4.531362</v>
+      </c>
+      <c r="E48" s="0" t="n">
+        <v>2.403149</v>
+      </c>
+      <c r="F48" s="0" t="n">
         <v>0.599600000000009</v>
       </c>
-      <c r="D48" s="0" t="n">
-        <v>6.1752</v>
-      </c>
-      <c r="E48" s="0" t="n">
+      <c r="G48" s="0" t="n">
         <v>0.800000000000068</v>
       </c>
-      <c r="F48" s="0" t="n">
-        <v>4.531362</v>
-      </c>
-      <c r="G48" s="0" t="n">
-        <v>78.6675</v>
-      </c>
       <c r="H48" s="0" t="n">
-        <v>2.403149</v>
+        <v>0.200500000000034</v>
       </c>
       <c r="I48" s="0" t="n">
         <v>3.59880000000001</v>
@@ -4853,22 +4853,22 @@
         <v>7.024949</v>
       </c>
       <c r="C49" s="0" t="n">
+        <v>10.71349</v>
+      </c>
+      <c r="D49" s="0" t="n">
+        <v>6.052003</v>
+      </c>
+      <c r="E49" s="0" t="n">
+        <v>6.231959</v>
+      </c>
+      <c r="F49" s="0" t="n">
         <v>7.26780000000008</v>
       </c>
-      <c r="D49" s="0" t="n">
-        <v>10.71349</v>
-      </c>
-      <c r="E49" s="0" t="n">
+      <c r="G49" s="0" t="n">
         <v>4.35579999999993</v>
       </c>
-      <c r="F49" s="0" t="n">
-        <v>6.052003</v>
-      </c>
-      <c r="G49" s="0" t="n">
+      <c r="H49" s="0" t="n">
         <v>2.55560000000003</v>
-      </c>
-      <c r="H49" s="0" t="n">
-        <v>6.231959</v>
       </c>
       <c r="I49" s="0" t="n">
         <v>3.2013</v>
@@ -4882,22 +4882,22 @@
         <v>5.138432</v>
       </c>
       <c r="C50" s="0" t="n">
-        <v>59.812</v>
+        <v>2.662827</v>
       </c>
       <c r="D50" s="0" t="n">
-        <v>2.662827</v>
+        <v>2.905388</v>
       </c>
       <c r="E50" s="0" t="n">
+        <v>0.8447551</v>
+      </c>
+      <c r="F50" s="0" t="n">
+        <v>9.32300000000009</v>
+      </c>
+      <c r="G50" s="0" t="n">
         <v>13.8996</v>
       </c>
-      <c r="F50" s="0" t="n">
-        <v>2.905388</v>
-      </c>
-      <c r="G50" s="0" t="n">
+      <c r="H50" s="0" t="n">
         <v>16.1048999999999</v>
-      </c>
-      <c r="H50" s="0" t="n">
-        <v>0.8447551</v>
       </c>
       <c r="I50" s="0" t="n">
         <v>14.35628</v>
@@ -4908,25 +4908,25 @@
         <v>4</v>
       </c>
       <c r="B51" s="0" t="n">
-        <v>3.513048</v>
+        <v>3.737296</v>
       </c>
       <c r="C51" s="0" t="n">
-        <v>-26.6199999999999</v>
+        <v>4.678463</v>
       </c>
       <c r="D51" s="0" t="n">
-        <v>4.678463</v>
+        <v>2.505874</v>
       </c>
       <c r="E51" s="0" t="n">
+        <v>1.187657</v>
+      </c>
+      <c r="F51" s="0" t="n">
+        <v>9.17000000000007</v>
+      </c>
+      <c r="G51" s="0" t="n">
         <v>7.25080000000003</v>
       </c>
-      <c r="F51" s="0" t="n">
-        <v>2.505874</v>
-      </c>
-      <c r="G51" s="0" t="n">
+      <c r="H51" s="0" t="n">
         <v>9.25400000000002</v>
-      </c>
-      <c r="H51" s="0" t="n">
-        <v>1.187657</v>
       </c>
       <c r="I51" s="0" t="n">
         <v>16.94954</v>
@@ -4937,25 +4937,25 @@
         <v>4</v>
       </c>
       <c r="B52" s="0" t="n">
-        <v>5.950465</v>
+        <v>6.744919</v>
       </c>
       <c r="C52" s="0" t="n">
-        <v>6.02499999999986</v>
+        <v>2.671921</v>
       </c>
       <c r="D52" s="0" t="n">
-        <v>2.671921</v>
+        <v>6.514083</v>
       </c>
       <c r="E52" s="0" t="n">
+        <v>5.204786</v>
+      </c>
+      <c r="F52" s="0" t="n">
+        <v>21.4349999999999</v>
+      </c>
+      <c r="G52" s="0" t="n">
         <v>12.4064</v>
       </c>
-      <c r="F52" s="0" t="n">
-        <v>6.514083</v>
-      </c>
-      <c r="G52" s="0" t="n">
+      <c r="H52" s="0" t="n">
         <v>5.05640000000005</v>
-      </c>
-      <c r="H52" s="0" t="n">
-        <v>5.204786</v>
       </c>
       <c r="I52" s="0" t="n">
         <v>4.6003</v>
@@ -4969,22 +4969,22 @@
         <v>2.334157</v>
       </c>
       <c r="C53" s="0" t="n">
-        <v>58.5710000000001</v>
+        <v>3.289769</v>
       </c>
       <c r="D53" s="0" t="n">
-        <v>3.289769</v>
+        <v>3.585242</v>
       </c>
       <c r="E53" s="0" t="n">
+        <v>1.972835</v>
+      </c>
+      <c r="F53" s="0" t="n">
+        <v>7.37100000000009</v>
+      </c>
+      <c r="G53" s="0" t="n">
         <v>3.55180000000007</v>
       </c>
-      <c r="F53" s="0" t="n">
-        <v>3.585242</v>
-      </c>
-      <c r="G53" s="0" t="n">
+      <c r="H53" s="0" t="n">
         <v>5.25459999999998</v>
-      </c>
-      <c r="H53" s="0" t="n">
-        <v>1.972835</v>
       </c>
       <c r="I53" s="0" t="n">
         <v>5.94999</v>
@@ -4998,22 +4998,22 @@
         <v>5.396384</v>
       </c>
       <c r="C54" s="0" t="n">
+        <v>5.157487</v>
+      </c>
+      <c r="D54" s="0" t="n">
+        <v>4.791326</v>
+      </c>
+      <c r="E54" s="0" t="n">
+        <v>1.700862</v>
+      </c>
+      <c r="F54" s="0" t="n">
         <v>6.52099999999996</v>
       </c>
-      <c r="D54" s="0" t="n">
-        <v>5.157487</v>
-      </c>
-      <c r="E54" s="0" t="n">
+      <c r="G54" s="0" t="n">
         <v>11.4552</v>
       </c>
-      <c r="F54" s="0" t="n">
-        <v>4.791326</v>
-      </c>
-      <c r="G54" s="0" t="n">
+      <c r="H54" s="0" t="n">
         <v>9.56129999999996</v>
-      </c>
-      <c r="H54" s="0" t="n">
-        <v>1.700862</v>
       </c>
       <c r="I54" s="0" t="n">
         <v>9.94886</v>
@@ -5027,22 +5027,22 @@
         <v>4.758465</v>
       </c>
       <c r="C55" s="0" t="n">
+        <v>5.459589</v>
+      </c>
+      <c r="D55" s="0" t="n">
+        <v>5.975333</v>
+      </c>
+      <c r="E55" s="0" t="n">
+        <v>2.832947</v>
+      </c>
+      <c r="F55" s="0" t="n">
         <v>2.20499999999993</v>
       </c>
-      <c r="D55" s="0" t="n">
-        <v>5.459589</v>
-      </c>
-      <c r="E55" s="0" t="n">
+      <c r="G55" s="0" t="n">
         <v>4.45280000000003</v>
       </c>
-      <c r="F55" s="0" t="n">
-        <v>5.975333</v>
-      </c>
-      <c r="G55" s="0" t="n">
+      <c r="H55" s="0" t="n">
         <v>2.60140000000001</v>
-      </c>
-      <c r="H55" s="0" t="n">
-        <v>2.832947</v>
       </c>
       <c r="I55" s="0" t="n">
         <v>12.10065</v>
@@ -5056,22 +5056,22 @@
         <v>3.129273</v>
       </c>
       <c r="C56" s="0" t="n">
+        <v>1.008682</v>
+      </c>
+      <c r="D56" s="0" t="n">
+        <v>4.743041</v>
+      </c>
+      <c r="E56" s="0" t="n">
+        <v>1.850782</v>
+      </c>
+      <c r="F56" s="0" t="n">
         <v>4.9670000000001</v>
       </c>
-      <c r="D56" s="0" t="n">
-        <v>1.008682</v>
-      </c>
-      <c r="E56" s="0" t="n">
+      <c r="G56" s="0" t="n">
         <v>2.40229999999997</v>
       </c>
-      <c r="F56" s="0" t="n">
-        <v>4.743041</v>
-      </c>
-      <c r="G56" s="0" t="n">
+      <c r="H56" s="0" t="n">
         <v>3.80370000000005</v>
-      </c>
-      <c r="H56" s="0" t="n">
-        <v>1.850782</v>
       </c>
       <c r="I56" s="0" t="n">
         <v>3.60055</v>
@@ -5085,22 +5085,22 @@
         <v>10.49073</v>
       </c>
       <c r="C57" s="0" t="n">
+        <v>9.78767</v>
+      </c>
+      <c r="D57" s="0" t="n">
+        <v>6.006238</v>
+      </c>
+      <c r="E57" s="0" t="n">
+        <v>2.717279</v>
+      </c>
+      <c r="F57" s="0" t="n">
         <v>2.45100000000002</v>
       </c>
-      <c r="D57" s="0" t="n">
-        <v>9.78767</v>
-      </c>
-      <c r="E57" s="0" t="n">
+      <c r="G57" s="0" t="n">
         <v>1.95090000000005</v>
       </c>
-      <c r="F57" s="0" t="n">
-        <v>6.006238</v>
-      </c>
-      <c r="G57" s="0" t="n">
+      <c r="H57" s="0" t="n">
         <v>2.30309999999997</v>
-      </c>
-      <c r="H57" s="0" t="n">
-        <v>2.717279</v>
       </c>
       <c r="I57" s="0" t="n">
         <v>3.09994</v>
@@ -5114,22 +5114,22 @@
         <v>3.045677</v>
       </c>
       <c r="C58" s="0" t="n">
+        <v>2.021696</v>
+      </c>
+      <c r="D58" s="0" t="n">
+        <v>1.32494</v>
+      </c>
+      <c r="E58" s="0" t="n">
+        <v>2.857258</v>
+      </c>
+      <c r="F58" s="0" t="n">
         <v>68.926</v>
       </c>
-      <c r="D58" s="0" t="n">
-        <v>2.021696</v>
-      </c>
-      <c r="E58" s="0" t="n">
+      <c r="G58" s="0" t="n">
         <v>3.132039</v>
       </c>
-      <c r="F58" s="0" t="n">
-        <v>1.32494</v>
-      </c>
-      <c r="G58" s="0" t="n">
+      <c r="H58" s="0" t="n">
         <v>16.1808000000001</v>
-      </c>
-      <c r="H58" s="0" t="n">
-        <v>2.857258</v>
       </c>
       <c r="I58" s="0" t="n">
         <v>16.99958</v>
@@ -5143,22 +5143,22 @@
         <v>5.004166</v>
       </c>
       <c r="C59" s="0" t="n">
+        <v>11.1561</v>
+      </c>
+      <c r="D59" s="0" t="n">
+        <v>1.276536</v>
+      </c>
+      <c r="E59" s="0" t="n">
+        <v>3.433657</v>
+      </c>
+      <c r="F59" s="0" t="n">
         <v>0.752900000000011</v>
       </c>
-      <c r="D59" s="0" t="n">
-        <v>11.1561</v>
-      </c>
-      <c r="E59" s="0" t="n">
+      <c r="G59" s="0" t="n">
         <v>1.00070000000005</v>
       </c>
-      <c r="F59" s="0" t="n">
-        <v>1.276536</v>
-      </c>
-      <c r="G59" s="0" t="n">
+      <c r="H59" s="0" t="n">
         <v>2.4511</v>
-      </c>
-      <c r="H59" s="0" t="n">
-        <v>3.433657</v>
       </c>
       <c r="I59" s="0" t="n">
         <v>1.35037</v>
@@ -5172,22 +5172,22 @@
         <v>8.576299</v>
       </c>
       <c r="C60" s="0" t="n">
+        <v>8.645294</v>
+      </c>
+      <c r="D60" s="0" t="n">
+        <v>3.357939</v>
+      </c>
+      <c r="E60" s="0" t="n">
+        <v>6.065219</v>
+      </c>
+      <c r="F60" s="0" t="n">
         <v>54.3346</v>
       </c>
-      <c r="D60" s="0" t="n">
-        <v>8.645294</v>
-      </c>
-      <c r="E60" s="0" t="n">
+      <c r="G60" s="0" t="n">
         <v>26.773</v>
       </c>
-      <c r="F60" s="0" t="n">
-        <v>3.357939</v>
-      </c>
-      <c r="G60" s="0" t="n">
+      <c r="H60" s="0" t="n">
         <v>15.6804000000001</v>
-      </c>
-      <c r="H60" s="0" t="n">
-        <v>6.065219</v>
       </c>
       <c r="I60" s="0" t="n">
         <v>13.25635</v>
@@ -5201,22 +5201,22 @@
         <v>6.292006</v>
       </c>
       <c r="C61" s="0" t="n">
+        <v>6.976802</v>
+      </c>
+      <c r="D61" s="0" t="n">
+        <v>3.056986</v>
+      </c>
+      <c r="E61" s="0" t="n">
+        <v>1.041057</v>
+      </c>
+      <c r="F61" s="0" t="n">
         <v>32.8033</v>
       </c>
-      <c r="D61" s="0" t="n">
-        <v>6.976802</v>
-      </c>
-      <c r="E61" s="0" t="n">
+      <c r="G61" s="0" t="n">
         <v>29.2631</v>
       </c>
-      <c r="F61" s="0" t="n">
-        <v>3.056986</v>
-      </c>
-      <c r="G61" s="0" t="n">
+      <c r="H61" s="0" t="n">
         <v>20.1344</v>
-      </c>
-      <c r="H61" s="0" t="n">
-        <v>1.041057</v>
       </c>
       <c r="I61" s="0" t="n">
         <v>6.89860000000002</v>
@@ -5230,22 +5230,22 @@
         <v>1.940643</v>
       </c>
       <c r="C62" s="0" t="n">
+        <v>2.859821</v>
+      </c>
+      <c r="D62" s="0" t="n">
+        <v>4.364777</v>
+      </c>
+      <c r="E62" s="0" t="n">
+        <v>2.634937</v>
+      </c>
+      <c r="F62" s="0" t="n">
         <v>27.5531999999999</v>
       </c>
-      <c r="D62" s="0" t="n">
-        <v>2.859821</v>
-      </c>
-      <c r="E62" s="0" t="n">
+      <c r="G62" s="0" t="n">
         <v>34.2887999999999</v>
       </c>
-      <c r="F62" s="0" t="n">
-        <v>4.364777</v>
-      </c>
-      <c r="G62" s="0" t="n">
+      <c r="H62" s="0" t="n">
         <v>12.5312</v>
-      </c>
-      <c r="H62" s="0" t="n">
-        <v>2.634937</v>
       </c>
       <c r="I62" s="0" t="n">
         <v>6.6497</v>
@@ -5259,22 +5259,22 @@
         <v>1.894127</v>
       </c>
       <c r="C63" s="0" t="n">
+        <v>6.039015</v>
+      </c>
+      <c r="D63" s="0" t="n">
+        <v>3.482063</v>
+      </c>
+      <c r="E63" s="0" t="n">
+        <v>5.505518</v>
+      </c>
+      <c r="F63" s="0" t="n">
         <v>67.4273000000001</v>
       </c>
-      <c r="D63" s="0" t="n">
-        <v>6.039015</v>
-      </c>
-      <c r="E63" s="0" t="n">
+      <c r="G63" s="0" t="n">
         <v>22.5372</v>
       </c>
-      <c r="F63" s="0" t="n">
-        <v>3.482063</v>
-      </c>
-      <c r="G63" s="0" t="n">
+      <c r="H63" s="0" t="n">
         <v>7.26459999999997</v>
-      </c>
-      <c r="H63" s="0" t="n">
-        <v>5.505518</v>
       </c>
       <c r="I63" s="0" t="n">
         <v>4.00129999999999</v>
@@ -5288,22 +5288,22 @@
         <v>2.947931</v>
       </c>
       <c r="C64" s="0" t="n">
+        <v>2.347402</v>
+      </c>
+      <c r="D64" s="0" t="n">
+        <v>0.7966306</v>
+      </c>
+      <c r="E64" s="0" t="n">
+        <v>1.319776</v>
+      </c>
+      <c r="F64" s="0" t="n">
         <v>69.2912</v>
       </c>
-      <c r="D64" s="0" t="n">
-        <v>2.347402</v>
-      </c>
-      <c r="E64" s="0" t="n">
+      <c r="G64" s="0" t="n">
         <v>21.0832</v>
       </c>
-      <c r="F64" s="0" t="n">
-        <v>0.7966306</v>
-      </c>
-      <c r="G64" s="0" t="n">
+      <c r="H64" s="0" t="n">
         <v>19.831</v>
-      </c>
-      <c r="H64" s="0" t="n">
-        <v>1.319776</v>
       </c>
       <c r="I64" s="0" t="n">
         <v>11.2039</v>
@@ -5317,22 +5317,22 @@
         <v>2.556393</v>
       </c>
       <c r="C65" s="0" t="n">
+        <v>6.170785</v>
+      </c>
+      <c r="D65" s="0" t="n">
+        <v>3.804438</v>
+      </c>
+      <c r="E65" s="0" t="n">
+        <v>5.834167</v>
+      </c>
+      <c r="F65" s="0" t="n">
         <v>14.0486999999999</v>
       </c>
-      <c r="D65" s="0" t="n">
-        <v>6.170785</v>
-      </c>
-      <c r="E65" s="0" t="n">
+      <c r="G65" s="0" t="n">
         <v>7.01220000000001</v>
       </c>
-      <c r="F65" s="0" t="n">
-        <v>3.804438</v>
-      </c>
-      <c r="G65" s="0" t="n">
+      <c r="H65" s="0" t="n">
         <v>8.21529999999996</v>
-      </c>
-      <c r="H65" s="0" t="n">
-        <v>5.834167</v>
       </c>
       <c r="I65" s="0" t="n">
         <v>7.0008</v>
@@ -5346,22 +5346,22 @@
         <v>2.599944</v>
       </c>
       <c r="C66" s="0" t="n">
+        <v>4.117507</v>
+      </c>
+      <c r="D66" s="0" t="n">
+        <v>2.000157</v>
+      </c>
+      <c r="E66" s="0" t="n">
+        <v>2.054172</v>
+      </c>
+      <c r="F66" s="0" t="n">
         <v>10.9284</v>
       </c>
-      <c r="D66" s="0" t="n">
-        <v>4.117507</v>
-      </c>
-      <c r="E66" s="0" t="n">
+      <c r="G66" s="0" t="n">
         <v>6.30640000000005</v>
       </c>
-      <c r="F66" s="0" t="n">
-        <v>2.000157</v>
-      </c>
-      <c r="G66" s="0" t="n">
+      <c r="H66" s="0" t="n">
         <v>0.759700000000066</v>
-      </c>
-      <c r="H66" s="0" t="n">
-        <v>2.054172</v>
       </c>
       <c r="I66" s="0" t="n">
         <v>2.29990000000001</v>
@@ -5375,22 +5375,22 @@
         <v>2.721511</v>
       </c>
       <c r="C67" s="0" t="n">
+        <v>1.728715</v>
+      </c>
+      <c r="D67" s="0" t="n">
+        <v>2.711778</v>
+      </c>
+      <c r="E67" s="0" t="n">
+        <v>1.97392</v>
+      </c>
+      <c r="F67" s="0" t="n">
         <v>28.0023</v>
       </c>
-      <c r="D67" s="0" t="n">
-        <v>1.728715</v>
-      </c>
-      <c r="E67" s="0" t="n">
+      <c r="G67" s="0" t="n">
         <v>13.6781999999999</v>
       </c>
-      <c r="F67" s="0" t="n">
-        <v>2.711778</v>
-      </c>
-      <c r="G67" s="0" t="n">
+      <c r="H67" s="0" t="n">
         <v>2.899</v>
-      </c>
-      <c r="H67" s="0" t="n">
-        <v>1.97392</v>
       </c>
       <c r="I67" s="0" t="n">
         <v>8.34999999999999</v>
@@ -5404,22 +5404,22 @@
         <v>5.779489</v>
       </c>
       <c r="C68" s="0" t="n">
+        <v>7.570924</v>
+      </c>
+      <c r="D68" s="0" t="n">
+        <v>5.216095</v>
+      </c>
+      <c r="E68" s="0" t="n">
+        <v>3.826589</v>
+      </c>
+      <c r="F68" s="0" t="n">
         <v>30.3333</v>
       </c>
-      <c r="D68" s="0" t="n">
-        <v>7.570924</v>
-      </c>
-      <c r="E68" s="0" t="n">
+      <c r="G68" s="0" t="n">
         <v>3.10739999999998</v>
       </c>
-      <c r="F68" s="0" t="n">
-        <v>5.216095</v>
-      </c>
-      <c r="G68" s="0" t="n">
+      <c r="H68" s="0" t="n">
         <v>12.7782999999999</v>
-      </c>
-      <c r="H68" s="0" t="n">
-        <v>3.826589</v>
       </c>
       <c r="I68" s="0" t="n">
         <v>8.6491</v>
@@ -5433,22 +5433,22 @@
         <v>7.508948</v>
       </c>
       <c r="C69" s="0" t="n">
+        <v>5.059011</v>
+      </c>
+      <c r="D69" s="0" t="n">
+        <v>6.387544</v>
+      </c>
+      <c r="E69" s="0" t="n">
+        <v>3.436184</v>
+      </c>
+      <c r="F69" s="0" t="n">
         <v>39.6673</v>
       </c>
-      <c r="D69" s="0" t="n">
-        <v>5.059011</v>
-      </c>
-      <c r="E69" s="0" t="n">
+      <c r="G69" s="0" t="n">
         <v>12.2635</v>
       </c>
-      <c r="F69" s="0" t="n">
-        <v>6.387544</v>
-      </c>
-      <c r="G69" s="0" t="n">
+      <c r="H69" s="0" t="n">
         <v>19.8903</v>
-      </c>
-      <c r="H69" s="0" t="n">
-        <v>3.436184</v>
       </c>
       <c r="I69" s="0" t="n">
         <v>18.0515</v>
@@ -5462,22 +5462,22 @@
         <v>1.595938</v>
       </c>
       <c r="C70" s="0" t="n">
+        <v>1.568244</v>
+      </c>
+      <c r="D70" s="0" t="n">
+        <v>3.28224</v>
+      </c>
+      <c r="E70" s="0" t="n">
+        <v>2.386374</v>
+      </c>
+      <c r="F70" s="0" t="n">
         <v>16.2774000000001</v>
       </c>
-      <c r="D70" s="0" t="n">
-        <v>1.568244</v>
-      </c>
-      <c r="E70" s="0" t="n">
+      <c r="G70" s="0" t="n">
         <v>15.6111</v>
       </c>
-      <c r="F70" s="0" t="n">
-        <v>3.28224</v>
-      </c>
-      <c r="G70" s="0" t="n">
+      <c r="H70" s="0" t="n">
         <v>10.7245</v>
-      </c>
-      <c r="H70" s="0" t="n">
-        <v>2.386374</v>
       </c>
       <c r="I70" s="0" t="n">
         <v>10.1507</v>
@@ -5491,22 +5491,22 @@
         <v>2.211048</v>
       </c>
       <c r="C71" s="0" t="n">
+        <v>2.054707</v>
+      </c>
+      <c r="D71" s="0" t="n">
+        <v>5.693509</v>
+      </c>
+      <c r="E71" s="0" t="n">
+        <v>5.690905</v>
+      </c>
+      <c r="F71" s="0" t="n">
         <v>66.0962999999999</v>
       </c>
-      <c r="D71" s="0" t="n">
-        <v>2.054707</v>
-      </c>
-      <c r="E71" s="0" t="n">
+      <c r="G71" s="0" t="n">
         <v>34.8908</v>
       </c>
-      <c r="F71" s="0" t="n">
-        <v>5.693509</v>
-      </c>
-      <c r="G71" s="0" t="n">
+      <c r="H71" s="0" t="n">
         <v>5.16679999999997</v>
-      </c>
-      <c r="H71" s="0" t="n">
-        <v>5.690905</v>
       </c>
       <c r="I71" s="0" t="n">
         <v>2.69920000000002</v>
@@ -5520,22 +5520,22 @@
         <v>1.685467</v>
       </c>
       <c r="C72" s="0" t="n">
+        <v>1.486511</v>
+      </c>
+      <c r="D72" s="0" t="n">
+        <v>4.536176</v>
+      </c>
+      <c r="E72" s="0" t="n">
+        <v>1.570691</v>
+      </c>
+      <c r="F72" s="0" t="n">
         <v>28.5598</v>
       </c>
-      <c r="D72" s="0" t="n">
-        <v>1.486511</v>
-      </c>
-      <c r="E72" s="0" t="n">
+      <c r="G72" s="0" t="n">
         <v>10.4122</v>
       </c>
-      <c r="F72" s="0" t="n">
-        <v>4.536176</v>
-      </c>
-      <c r="G72" s="0" t="n">
+      <c r="H72" s="0" t="n">
         <v>10.3151</v>
-      </c>
-      <c r="H72" s="0" t="n">
-        <v>1.570691</v>
       </c>
       <c r="I72" s="0" t="n">
         <v>15.707</v>
@@ -5549,22 +5549,22 @@
         <v>1.625238</v>
       </c>
       <c r="C73" s="0" t="n">
+        <v>2.935864</v>
+      </c>
+      <c r="D73" s="0" t="n">
+        <v>0.9291179</v>
+      </c>
+      <c r="E73" s="0" t="n">
+        <v>5.098012</v>
+      </c>
+      <c r="F73" s="0" t="n">
         <v>20.2879</v>
       </c>
-      <c r="D73" s="0" t="n">
-        <v>2.935864</v>
-      </c>
-      <c r="E73" s="0" t="n">
+      <c r="G73" s="0" t="n">
         <v>10.0148</v>
       </c>
-      <c r="F73" s="0" t="n">
-        <v>0.9291179</v>
-      </c>
-      <c r="G73" s="0" t="n">
+      <c r="H73" s="0" t="n">
         <v>9.32280000000003</v>
-      </c>
-      <c r="H73" s="0" t="n">
-        <v>5.098012</v>
       </c>
       <c r="I73" s="0" t="n">
         <v>5.69869999999997</v>
@@ -5578,22 +5578,22 @@
         <v>3.956848</v>
       </c>
       <c r="C74" s="0" t="n">
+        <v>3.661891</v>
+      </c>
+      <c r="D74" s="0" t="n">
+        <v>4.633134</v>
+      </c>
+      <c r="E74" s="0" t="n">
+        <v>2.467311</v>
+      </c>
+      <c r="F74" s="0" t="n">
         <v>5.27539999999999</v>
       </c>
-      <c r="D74" s="0" t="n">
-        <v>3.661891</v>
-      </c>
-      <c r="E74" s="0" t="n">
+      <c r="G74" s="0" t="n">
         <v>15.2748</v>
       </c>
-      <c r="F74" s="0" t="n">
-        <v>4.633134</v>
-      </c>
-      <c r="G74" s="0" t="n">
+      <c r="H74" s="0" t="n">
         <v>1.06549999999993</v>
-      </c>
-      <c r="H74" s="0" t="n">
-        <v>2.467311</v>
       </c>
       <c r="I74" s="0" t="n">
         <v>2.19980000000004</v>
@@ -5607,22 +5607,22 @@
         <v>3.579314</v>
       </c>
       <c r="C75" s="0" t="n">
+        <v>2.148463</v>
+      </c>
+      <c r="D75" s="0" t="n">
+        <v>3.51844</v>
+      </c>
+      <c r="E75" s="0" t="n">
+        <v>2.309717</v>
+      </c>
+      <c r="F75" s="0" t="n">
         <v>17.2543000000001</v>
       </c>
-      <c r="D75" s="0" t="n">
-        <v>2.148463</v>
-      </c>
-      <c r="E75" s="0" t="n">
+      <c r="G75" s="0" t="n">
         <v>7.01139999999998</v>
       </c>
-      <c r="F75" s="0" t="n">
-        <v>3.51844</v>
-      </c>
-      <c r="G75" s="0" t="n">
+      <c r="H75" s="0" t="n">
         <v>0.149200000000064</v>
-      </c>
-      <c r="H75" s="0" t="n">
-        <v>2.309717</v>
       </c>
       <c r="I75" s="0" t="n">
         <v>0.551599999999951</v>
@@ -5636,22 +5636,22 @@
         <v>4.234471</v>
       </c>
       <c r="C76" s="0" t="n">
+        <v>10.74802</v>
+      </c>
+      <c r="D76" s="0" t="n">
+        <v>5.00279</v>
+      </c>
+      <c r="E76" s="0" t="n">
+        <v>3.10129</v>
+      </c>
+      <c r="F76" s="0" t="n">
         <v>30.082</v>
       </c>
-      <c r="D76" s="0" t="n">
-        <v>10.74802</v>
-      </c>
-      <c r="E76" s="0" t="n">
+      <c r="G76" s="0" t="n">
         <v>3.80629999999996</v>
       </c>
-      <c r="F76" s="0" t="n">
-        <v>5.00279</v>
-      </c>
-      <c r="G76" s="0" t="n">
+      <c r="H76" s="0" t="n">
         <v>3.91049999999996</v>
-      </c>
-      <c r="H76" s="0" t="n">
-        <v>3.10129</v>
       </c>
       <c r="I76" s="0" t="n">
         <v>8.30119999999999</v>
@@ -5665,18 +5665,18 @@
         <v>2.285027</v>
       </c>
       <c r="C77" s="0" t="n">
+        <v>4.66028</v>
+      </c>
+      <c r="D77" s="0" t="n">
+        <v>1.85473</v>
+      </c>
+      <c r="F77" s="0" t="n">
         <v>28.547</v>
       </c>
-      <c r="D77" s="0" t="n">
-        <v>4.66028</v>
-      </c>
-      <c r="E77" s="0" t="n">
+      <c r="G77" s="0" t="n">
         <v>58.2354</v>
       </c>
-      <c r="F77" s="0" t="n">
-        <v>1.85473</v>
-      </c>
-      <c r="G77" s="0" t="n">
+      <c r="H77" s="0" t="n">
         <v>17.00445</v>
       </c>
     </row>
@@ -5688,18 +5688,18 @@
         <v>6.62722</v>
       </c>
       <c r="C78" s="0" t="n">
+        <v>4.543006</v>
+      </c>
+      <c r="D78" s="0" t="n">
+        <v>2.875784</v>
+      </c>
+      <c r="F78" s="0" t="n">
         <v>0.799900000000037</v>
       </c>
-      <c r="D78" s="0" t="n">
-        <v>4.543006</v>
-      </c>
-      <c r="E78" s="0" t="n">
+      <c r="G78" s="0" t="n">
         <v>0.549300000000017</v>
       </c>
-      <c r="F78" s="0" t="n">
-        <v>2.875784</v>
-      </c>
-      <c r="G78" s="0" t="n">
+      <c r="H78" s="0" t="n">
         <v>1.00108</v>
       </c>
     </row>
@@ -5711,18 +5711,18 @@
         <v>9.002918</v>
       </c>
       <c r="C79" s="0" t="n">
+        <v>8.891509</v>
+      </c>
+      <c r="D79" s="0" t="n">
+        <v>4.309965</v>
+      </c>
+      <c r="F79" s="0" t="n">
         <v>39.7952</v>
       </c>
-      <c r="D79" s="0" t="n">
-        <v>8.891509</v>
-      </c>
-      <c r="E79" s="0" t="n">
+      <c r="G79" s="0" t="n">
         <v>16.0269</v>
       </c>
-      <c r="F79" s="0" t="n">
-        <v>4.309965</v>
-      </c>
-      <c r="G79" s="0" t="n">
+      <c r="H79" s="0" t="n">
         <v>23.2995</v>
       </c>
     </row>
@@ -5731,21 +5731,21 @@
         <v>3</v>
       </c>
       <c r="B80" s="0" t="n">
-        <v>3.697272</v>
+        <v>10.34307</v>
       </c>
       <c r="C80" s="0" t="n">
-        <v>17.4450999999999</v>
+        <v>6.838632</v>
       </c>
       <c r="D80" s="0" t="n">
-        <v>3.971377</v>
-      </c>
-      <c r="E80" s="0" t="n">
-        <v>35.3665999999999</v>
+        <v>5.685935</v>
       </c>
       <c r="F80" s="0" t="n">
-        <v>5.685935</v>
+        <v>28.7244999999999</v>
       </c>
       <c r="G80" s="0" t="n">
+        <v>18.4039</v>
+      </c>
+      <c r="H80" s="0" t="n">
         <v>35.1</v>
       </c>
     </row>
@@ -5757,18 +5757,18 @@
         <v>6.275187</v>
       </c>
       <c r="C81" s="0" t="n">
-        <v>117.2078</v>
+        <v>3.861755</v>
       </c>
       <c r="D81" s="0" t="n">
-        <v>3.118359</v>
-      </c>
-      <c r="E81" s="0" t="n">
-        <v>13.186</v>
+        <v>1.319708</v>
       </c>
       <c r="F81" s="0" t="n">
-        <v>1.319708</v>
+        <v>21.0163</v>
       </c>
       <c r="G81" s="0" t="n">
+        <v>17.486</v>
+      </c>
+      <c r="H81" s="0" t="n">
         <v>63.4815</v>
       </c>
     </row>
@@ -5780,18 +5780,18 @@
         <v>6.146957</v>
       </c>
       <c r="C82" s="0" t="n">
+        <v>5.753842</v>
+      </c>
+      <c r="D82" s="0" t="n">
+        <v>1.291296</v>
+      </c>
+      <c r="F82" s="0" t="n">
         <v>31.7570000000001</v>
       </c>
-      <c r="D82" s="0" t="n">
-        <v>3.838295</v>
-      </c>
-      <c r="E82" s="0" t="n">
-        <v>16.1315999999999</v>
-      </c>
-      <c r="F82" s="0" t="n">
-        <v>1.291296</v>
-      </c>
       <c r="G82" s="0" t="n">
+        <v>27.9196999999999</v>
+      </c>
+      <c r="H82" s="0" t="n">
         <v>45.2247</v>
       </c>
     </row>
@@ -5803,18 +5803,18 @@
         <v>8.465077</v>
       </c>
       <c r="C83" s="0" t="n">
+        <v>2.178203</v>
+      </c>
+      <c r="D83" s="0" t="n">
+        <v>2.04324</v>
+      </c>
+      <c r="F83" s="0" t="n">
         <v>2.4665</v>
       </c>
-      <c r="D83" s="0" t="n">
-        <v>2.178203</v>
-      </c>
-      <c r="E83" s="0" t="n">
-        <v>98.2145</v>
-      </c>
-      <c r="F83" s="0" t="n">
-        <v>2.04324</v>
-      </c>
       <c r="G83" s="0" t="n">
+        <v>6.47810000000004</v>
+      </c>
+      <c r="H83" s="0" t="n">
         <v>63.3952</v>
       </c>
     </row>
@@ -5826,18 +5826,18 @@
         <v>4.289544</v>
       </c>
       <c r="C84" s="0" t="n">
+        <v>5.298734</v>
+      </c>
+      <c r="D84" s="0" t="n">
+        <v>3.313668</v>
+      </c>
+      <c r="F84" s="0" t="n">
         <v>1.75209999999993</v>
       </c>
-      <c r="D84" s="0" t="n">
-        <v>5.298734</v>
-      </c>
-      <c r="E84" s="0" t="n">
+      <c r="G84" s="0" t="n">
         <v>28.2796</v>
       </c>
-      <c r="F84" s="0" t="n">
-        <v>3.313668</v>
-      </c>
-      <c r="G84" s="0" t="n">
+      <c r="H84" s="0" t="n">
         <v>27.5784</v>
       </c>
     </row>
@@ -5849,18 +5849,18 @@
         <v>4.493312</v>
       </c>
       <c r="C85" s="0" t="n">
+        <v>4.905343</v>
+      </c>
+      <c r="D85" s="0" t="n">
+        <v>1.136087</v>
+      </c>
+      <c r="F85" s="0" t="n">
         <v>12.022</v>
       </c>
-      <c r="D85" s="0" t="n">
-        <v>4.905343</v>
-      </c>
-      <c r="E85" s="0" t="n">
+      <c r="G85" s="0" t="n">
         <v>6.41640000000007</v>
       </c>
-      <c r="F85" s="0" t="n">
-        <v>1.136087</v>
-      </c>
-      <c r="G85" s="0" t="n">
+      <c r="H85" s="0" t="n">
         <v>13.1628</v>
       </c>
     </row>
@@ -5872,18 +5872,18 @@
         <v>8.564166</v>
       </c>
       <c r="C86" s="0" t="n">
+        <v>4.51594</v>
+      </c>
+      <c r="D86" s="0" t="n">
+        <v>0.8041273</v>
+      </c>
+      <c r="F86" s="0" t="n">
         <v>3.90350000000001</v>
       </c>
-      <c r="D86" s="0" t="n">
-        <v>4.51594</v>
-      </c>
-      <c r="E86" s="0" t="n">
+      <c r="G86" s="0" t="n">
         <v>0.899299999999926</v>
       </c>
-      <c r="F86" s="0" t="n">
-        <v>0.8041273</v>
-      </c>
-      <c r="G86" s="0" t="n">
+      <c r="H86" s="0" t="n">
         <v>12.7676</v>
       </c>
     </row>
@@ -5895,18 +5895,18 @@
         <v>12.60928</v>
       </c>
       <c r="C87" s="0" t="n">
+        <v>7.221645</v>
+      </c>
+      <c r="D87" s="0" t="n">
+        <v>5.623559</v>
+      </c>
+      <c r="F87" s="0" t="n">
         <v>4.0136</v>
       </c>
-      <c r="D87" s="0" t="n">
-        <v>7.221645</v>
-      </c>
-      <c r="E87" s="0" t="n">
+      <c r="G87" s="0" t="n">
         <v>3.6504000000001</v>
       </c>
-      <c r="F87" s="0" t="n">
-        <v>5.623559</v>
-      </c>
-      <c r="G87" s="0" t="n">
+      <c r="H87" s="0" t="n">
         <v>19.0118</v>
       </c>
     </row>
@@ -5918,18 +5918,18 @@
         <v>13.06937</v>
       </c>
       <c r="C88" s="0" t="n">
+        <v>4.120884</v>
+      </c>
+      <c r="D88" s="0" t="n">
+        <v>4.070271</v>
+      </c>
+      <c r="F88" s="0" t="n">
         <v>56.9718</v>
       </c>
-      <c r="D88" s="0" t="n">
-        <v>4.120884</v>
-      </c>
-      <c r="E88" s="0" t="n">
+      <c r="G88" s="0" t="n">
         <v>21.6439</v>
       </c>
-      <c r="F88" s="0" t="n">
-        <v>4.070271</v>
-      </c>
-      <c r="G88" s="0" t="n">
+      <c r="H88" s="0" t="n">
         <v>37.617</v>
       </c>
     </row>
@@ -5941,18 +5941,18 @@
         <v>4.677553</v>
       </c>
       <c r="C89" s="0" t="n">
+        <v>2.494468</v>
+      </c>
+      <c r="D89" s="0" t="n">
+        <v>2.112444</v>
+      </c>
+      <c r="F89" s="0" t="n">
         <v>28.1351999999999</v>
       </c>
-      <c r="D89" s="0" t="n">
-        <v>2.494468</v>
-      </c>
-      <c r="E89" s="0" t="n">
+      <c r="G89" s="0" t="n">
         <v>14.3738</v>
       </c>
-      <c r="F89" s="0" t="n">
-        <v>2.112444</v>
-      </c>
-      <c r="G89" s="0" t="n">
+      <c r="H89" s="0" t="n">
         <v>18.4442</v>
       </c>
     </row>
@@ -5964,18 +5964,18 @@
         <v>8.41391</v>
       </c>
       <c r="C90" s="0" t="n">
+        <v>6.286272</v>
+      </c>
+      <c r="D90" s="0" t="n">
+        <v>3.681955</v>
+      </c>
+      <c r="F90" s="0" t="n">
         <v>15.1747</v>
       </c>
-      <c r="D90" s="0" t="n">
-        <v>6.286272</v>
-      </c>
-      <c r="E90" s="0" t="n">
+      <c r="G90" s="0" t="n">
         <v>4.96580000000006</v>
       </c>
-      <c r="F90" s="0" t="n">
-        <v>3.681955</v>
-      </c>
-      <c r="G90" s="0" t="n">
+      <c r="H90" s="0" t="n">
         <v>35.5512</v>
       </c>
     </row>
@@ -5987,18 +5987,18 @@
         <v>5.08027</v>
       </c>
       <c r="C91" s="0" t="n">
+        <v>3.316641</v>
+      </c>
+      <c r="D91" s="0" t="n">
+        <v>1.705178</v>
+      </c>
+      <c r="F91" s="0" t="n">
         <v>20.4458</v>
       </c>
-      <c r="D91" s="0" t="n">
-        <v>3.316641</v>
-      </c>
-      <c r="E91" s="0" t="n">
+      <c r="G91" s="0" t="n">
         <v>17.7370999999999</v>
       </c>
-      <c r="F91" s="0" t="n">
-        <v>1.705178</v>
-      </c>
-      <c r="G91" s="0" t="n">
+      <c r="H91" s="0" t="n">
         <v>45.9558999999999</v>
       </c>
     </row>
@@ -6010,18 +6010,18 @@
         <v>6.317364</v>
       </c>
       <c r="C92" s="0" t="n">
+        <v>9.288054</v>
+      </c>
+      <c r="D92" s="0" t="n">
+        <v>2.044359</v>
+      </c>
+      <c r="F92" s="0" t="n">
         <v>5.46699999999998</v>
       </c>
-      <c r="D92" s="0" t="n">
-        <v>9.288054</v>
-      </c>
-      <c r="E92" s="0" t="n">
+      <c r="G92" s="0" t="n">
         <v>11.5772000000001</v>
       </c>
-      <c r="F92" s="0" t="n">
-        <v>2.044359</v>
-      </c>
-      <c r="G92" s="0" t="n">
+      <c r="H92" s="0" t="n">
         <v>17.9100000000001</v>
       </c>
     </row>
@@ -6033,18 +6033,18 @@
         <v>6.680809</v>
       </c>
       <c r="C93" s="0" t="n">
+        <v>6.163433</v>
+      </c>
+      <c r="D93" s="0" t="n">
+        <v>2.427228</v>
+      </c>
+      <c r="F93" s="0" t="n">
         <v>9.82760000000008</v>
       </c>
-      <c r="D93" s="0" t="n">
-        <v>6.163433</v>
-      </c>
-      <c r="E93" s="0" t="n">
+      <c r="G93" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F93" s="0" t="n">
-        <v>2.427228</v>
-      </c>
-      <c r="G93" s="0" t="n">
+      <c r="H93" s="0" t="n">
         <v>7.11619999999994</v>
       </c>
     </row>
@@ -6056,18 +6056,18 @@
         <v>7.181819</v>
       </c>
       <c r="C94" s="0" t="n">
+        <v>6.00932</v>
+      </c>
+      <c r="D94" s="0" t="n">
+        <v>2.943125</v>
+      </c>
+      <c r="F94" s="0" t="n">
         <v>0.659099999999967</v>
       </c>
-      <c r="D94" s="0" t="n">
-        <v>6.00932</v>
-      </c>
-      <c r="E94" s="0" t="n">
+      <c r="G94" s="0" t="n">
         <v>2.69909999999993</v>
       </c>
-      <c r="F94" s="0" t="n">
-        <v>2.943125</v>
-      </c>
-      <c r="G94" s="0" t="n">
+      <c r="H94" s="0" t="n">
         <v>6.86390000000006</v>
       </c>
     </row>
@@ -6079,18 +6079,18 @@
         <v>16.22197</v>
       </c>
       <c r="C95" s="0" t="n">
+        <v>6.646376</v>
+      </c>
+      <c r="D95" s="0" t="n">
+        <v>4.643414</v>
+      </c>
+      <c r="F95" s="0" t="n">
         <v>1.65269999999998</v>
       </c>
-      <c r="D95" s="0" t="n">
-        <v>6.646376</v>
-      </c>
-      <c r="E95" s="0" t="n">
+      <c r="G95" s="0" t="n">
         <v>8.86980000000006</v>
       </c>
-      <c r="F95" s="0" t="n">
-        <v>4.643414</v>
-      </c>
-      <c r="G95" s="0" t="n">
+      <c r="H95" s="0" t="n">
         <v>20.2664</v>
       </c>
     </row>
@@ -6098,16 +6098,16 @@
       <c r="A96" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="C96" s="0" t="n">
+        <v>0.824275</v>
+      </c>
       <c r="D96" s="0" t="n">
-        <v>0.824275</v>
-      </c>
-      <c r="E96" s="0" t="n">
+        <v>2.160964</v>
+      </c>
+      <c r="G96" s="0" t="n">
         <v>31.55002</v>
       </c>
-      <c r="F96" s="0" t="n">
-        <v>2.160964</v>
-      </c>
-      <c r="G96" s="0" t="n">
+      <c r="H96" s="0" t="n">
         <v>21.1519999999999</v>
       </c>
     </row>
@@ -6115,16 +6115,16 @@
       <c r="A97" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="C97" s="0" t="n">
+        <v>1.957609</v>
+      </c>
       <c r="D97" s="0" t="n">
-        <v>1.957609</v>
-      </c>
-      <c r="E97" s="0" t="n">
+        <v>2.21305</v>
+      </c>
+      <c r="G97" s="0" t="n">
         <v>1.05002</v>
       </c>
-      <c r="F97" s="0" t="n">
-        <v>2.21305</v>
-      </c>
-      <c r="G97" s="0" t="n">
+      <c r="H97" s="0" t="n">
         <v>0.899600000000078</v>
       </c>
     </row>
@@ -6132,16 +6132,16 @@
       <c r="A98" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="C98" s="0" t="n">
+        <v>4.142436</v>
+      </c>
       <c r="D98" s="0" t="n">
-        <v>4.142436</v>
-      </c>
-      <c r="E98" s="0" t="n">
+        <v>8.903512</v>
+      </c>
+      <c r="G98" s="0" t="n">
         <v>32.00074</v>
       </c>
-      <c r="F98" s="0" t="n">
-        <v>8.903512</v>
-      </c>
-      <c r="G98" s="0" t="n">
+      <c r="H98" s="0" t="n">
         <v>37.5452</v>
       </c>
     </row>
@@ -6149,16 +6149,16 @@
       <c r="A99" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="C99" s="0" t="n">
+        <v>2.912466</v>
+      </c>
       <c r="D99" s="0" t="n">
-        <v>2.912466</v>
-      </c>
-      <c r="E99" s="0" t="n">
+        <v>5.691941</v>
+      </c>
+      <c r="G99" s="0" t="n">
         <v>15.8093</v>
       </c>
-      <c r="F99" s="0" t="n">
-        <v>5.691941</v>
-      </c>
-      <c r="G99" s="0" t="n">
+      <c r="H99" s="0" t="n">
         <v>11.4713</v>
       </c>
     </row>
@@ -6166,16 +6166,16 @@
       <c r="A100" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="C100" s="0" t="n">
+        <v>5.295904</v>
+      </c>
       <c r="D100" s="0" t="n">
-        <v>5.295904</v>
-      </c>
-      <c r="E100" s="0" t="n">
+        <v>3.181421</v>
+      </c>
+      <c r="G100" s="0" t="n">
         <v>12.65</v>
       </c>
-      <c r="F100" s="0" t="n">
-        <v>3.181421</v>
-      </c>
-      <c r="G100" s="0" t="n">
+      <c r="H100" s="0" t="n">
         <v>9.08309999999995</v>
       </c>
     </row>
@@ -6183,16 +6183,16 @@
       <c r="A101" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="C101" s="0" t="n">
+        <v>4.895791</v>
+      </c>
       <c r="D101" s="0" t="n">
-        <v>4.895791</v>
-      </c>
-      <c r="E101" s="0" t="n">
+        <v>6.379659</v>
+      </c>
+      <c r="G101" s="0" t="n">
         <v>10.9001</v>
       </c>
-      <c r="F101" s="0" t="n">
-        <v>6.379659</v>
-      </c>
-      <c r="G101" s="0" t="n">
+      <c r="H101" s="0" t="n">
         <v>7.11390000000006</v>
       </c>
     </row>
@@ -6200,16 +6200,16 @@
       <c r="A102" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="C102" s="0" t="n">
+        <v>2.943974</v>
+      </c>
       <c r="D102" s="0" t="n">
-        <v>2.943974</v>
-      </c>
-      <c r="E102" s="0" t="n">
+        <v>4.963771</v>
+      </c>
+      <c r="G102" s="0" t="n">
         <v>19.96</v>
       </c>
-      <c r="F102" s="0" t="n">
-        <v>4.963771</v>
-      </c>
-      <c r="G102" s="0" t="n">
+      <c r="H102" s="0" t="n">
         <v>4.90729999999996</v>
       </c>
     </row>
@@ -6217,16 +6217,16 @@
       <c r="A103" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="C103" s="0" t="n">
+        <v>4.568118</v>
+      </c>
       <c r="D103" s="0" t="n">
-        <v>4.568118</v>
-      </c>
-      <c r="E103" s="0" t="n">
+        <v>3.874757</v>
+      </c>
+      <c r="G103" s="0" t="n">
         <v>17.4616</v>
       </c>
-      <c r="F103" s="0" t="n">
-        <v>3.874757</v>
-      </c>
-      <c r="G103" s="0" t="n">
+      <c r="H103" s="0" t="n">
         <v>1.05029999999999</v>
       </c>
     </row>
@@ -6234,16 +6234,16 @@
       <c r="A104" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="C104" s="0" t="n">
+        <v>3.841986</v>
+      </c>
       <c r="D104" s="0" t="n">
-        <v>3.841986</v>
-      </c>
-      <c r="E104" s="0" t="n">
+        <v>3.732283</v>
+      </c>
+      <c r="G104" s="0" t="n">
         <v>10.2995</v>
       </c>
-      <c r="F104" s="0" t="n">
-        <v>3.732283</v>
-      </c>
-      <c r="G104" s="0" t="n">
+      <c r="H104" s="0" t="n">
         <v>0.350000000000023</v>
       </c>
     </row>
@@ -6251,16 +6251,16 @@
       <c r="A105" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="C105" s="0" t="n">
+        <v>3.190487</v>
+      </c>
       <c r="D105" s="0" t="n">
-        <v>3.190487</v>
-      </c>
-      <c r="E105" s="0" t="n">
+        <v>3.599788</v>
+      </c>
+      <c r="G105" s="0" t="n">
         <v>7.3999</v>
       </c>
-      <c r="F105" s="0" t="n">
-        <v>3.599788</v>
-      </c>
-      <c r="G105" s="0" t="n">
+      <c r="H105" s="0" t="n">
         <v>2.76310000000001</v>
       </c>
     </row>
@@ -6268,16 +6268,16 @@
       <c r="A106" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="C106" s="0" t="n">
+        <v>9.949568</v>
+      </c>
       <c r="D106" s="0" t="n">
-        <v>9.949568</v>
-      </c>
-      <c r="E106" s="0" t="n">
+        <v>6.805555</v>
+      </c>
+      <c r="G106" s="0" t="n">
         <v>3.69970000000001</v>
       </c>
-      <c r="F106" s="0" t="n">
-        <v>6.805555</v>
-      </c>
-      <c r="G106" s="0" t="n">
+      <c r="H106" s="0" t="n">
         <v>3.25779999999997</v>
       </c>
     </row>
@@ -6285,16 +6285,16 @@
       <c r="A107" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="C107" s="0" t="n">
+        <v>4.130274</v>
+      </c>
       <c r="D107" s="0" t="n">
-        <v>4.130274</v>
-      </c>
-      <c r="E107" s="0" t="n">
+        <v>7.322898</v>
+      </c>
+      <c r="G107" s="0" t="n">
         <v>16.25</v>
       </c>
-      <c r="F107" s="0" t="n">
-        <v>7.322898</v>
-      </c>
-      <c r="G107" s="0" t="n">
+      <c r="H107" s="0" t="n">
         <v>11.3672</v>
       </c>
     </row>
@@ -6302,16 +6302,16 @@
       <c r="A108" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="C108" s="0" t="n">
+        <v>1.674702</v>
+      </c>
       <c r="D108" s="0" t="n">
-        <v>1.674702</v>
-      </c>
-      <c r="E108" s="0" t="n">
+        <v>3.655144</v>
+      </c>
+      <c r="G108" s="0" t="n">
         <v>20.5003</v>
       </c>
-      <c r="F108" s="0" t="n">
-        <v>3.655144</v>
-      </c>
-      <c r="G108" s="0" t="n">
+      <c r="H108" s="0" t="n">
         <v>4.0557</v>
       </c>
     </row>
@@ -6319,16 +6319,16 @@
       <c r="A109" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="C109" s="0" t="n">
+        <v>5.980261</v>
+      </c>
       <c r="D109" s="0" t="n">
-        <v>5.980261</v>
-      </c>
-      <c r="E109" s="0" t="n">
+        <v>4.866443</v>
+      </c>
+      <c r="G109" s="0" t="n">
         <v>7.65109999999999</v>
       </c>
-      <c r="F109" s="0" t="n">
-        <v>4.866443</v>
-      </c>
-      <c r="G109" s="0" t="n">
+      <c r="H109" s="0" t="n">
         <v>4.61329999999998</v>
       </c>
     </row>
@@ -6336,16 +6336,16 @@
       <c r="A110" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="C110" s="0" t="n">
+        <v>1.211287</v>
+      </c>
       <c r="D110" s="0" t="n">
-        <v>1.211287</v>
-      </c>
-      <c r="E110" s="0" t="n">
+        <v>2.120363</v>
+      </c>
+      <c r="G110" s="0" t="n">
         <v>18.9631</v>
       </c>
-      <c r="F110" s="0" t="n">
-        <v>2.120363</v>
-      </c>
-      <c r="G110" s="0" t="n">
+      <c r="H110" s="0" t="n">
         <v>0.899099999999976</v>
       </c>
     </row>
@@ -6353,16 +6353,16 @@
       <c r="A111" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="C111" s="0" t="n">
+        <v>2.099525</v>
+      </c>
       <c r="D111" s="0" t="n">
-        <v>2.099525</v>
-      </c>
-      <c r="E111" s="0" t="n">
+        <v>3.561687</v>
+      </c>
+      <c r="G111" s="0" t="n">
         <v>13.7497</v>
       </c>
-      <c r="F111" s="0" t="n">
-        <v>3.561687</v>
-      </c>
-      <c r="G111" s="0" t="n">
+      <c r="H111" s="0" t="n">
         <v>12.1738</v>
       </c>
     </row>
@@ -6370,16 +6370,16 @@
       <c r="A112" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="C112" s="0" t="n">
+        <v>5.970841</v>
+      </c>
       <c r="D112" s="0" t="n">
-        <v>5.970841</v>
-      </c>
-      <c r="E112" s="0" t="n">
+        <v>4.607451</v>
+      </c>
+      <c r="G112" s="0" t="n">
         <v>3.64940000000001</v>
       </c>
-      <c r="F112" s="0" t="n">
-        <v>4.607451</v>
-      </c>
-      <c r="G112" s="0" t="n">
+      <c r="H112" s="0" t="n">
         <v>0.650300000000016</v>
       </c>
     </row>
@@ -6387,16 +6387,16 @@
       <c r="A113" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="C113" s="0" t="n">
+        <v>5.386072</v>
+      </c>
       <c r="D113" s="0" t="n">
-        <v>5.386072</v>
-      </c>
-      <c r="E113" s="0" t="n">
+        <v>3.627673</v>
+      </c>
+      <c r="G113" s="0" t="n">
         <v>6.55079999999998</v>
       </c>
-      <c r="F113" s="0" t="n">
-        <v>3.627673</v>
-      </c>
-      <c r="G113" s="0" t="n">
+      <c r="H113" s="0" t="n">
         <v>1.05729999999994</v>
       </c>
     </row>
@@ -6404,393 +6404,750 @@
       <c r="A114" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="C114" s="0" t="n">
+        <v>6.827086</v>
+      </c>
       <c r="D114" s="0" t="n">
-        <v>6.827086</v>
-      </c>
-      <c r="E114" s="0" t="n">
+        <v>6.910149</v>
+      </c>
+      <c r="G114" s="0" t="n">
         <v>4.59999999999997</v>
       </c>
-      <c r="F114" s="0" t="n">
-        <v>6.910149</v>
-      </c>
-      <c r="G114" s="0" t="n">
+      <c r="H114" s="0" t="n">
         <v>2.649</v>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C115" s="0" t="n">
+        <v>1.383808</v>
+      </c>
+      <c r="D115" s="0" t="n">
+        <v>2.554546</v>
+      </c>
+      <c r="G115" s="0" t="n">
+        <v>29.4053</v>
+      </c>
+      <c r="H115" s="0" t="n">
+        <v>41.1028</v>
+      </c>
+    </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="0" t="s">
+      <c r="A116" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B116" s="0" t="n">
-        <f aca="false">AVERAGE(B1:B114)</f>
-        <v>6.30904645263158</v>
-      </c>
       <c r="C116" s="0" t="n">
-        <f aca="false">AVERAGE(C1:C114)</f>
-        <v>20.1897115789474</v>
+        <v>2.91806</v>
       </c>
       <c r="D116" s="0" t="n">
-        <f aca="false">AVERAGE(D1:D114)</f>
-        <v>4.53520138571429</v>
-      </c>
-      <c r="E116" s="0" t="n">
-        <f aca="false">AVERAGE(E1:E114)</f>
-        <v>13.2883219553571</v>
-      </c>
-      <c r="F116" s="0" t="n">
-        <f aca="false">AVERAGE(F1:F114)</f>
-        <v>3.58695131403509</v>
+        <v>2.685068</v>
       </c>
       <c r="G116" s="0" t="n">
-        <f aca="false">AVERAGE(G1:G114)</f>
-        <v>14.8849842982456</v>
+        <v>10.0578</v>
       </c>
       <c r="H116" s="0" t="n">
-        <f aca="false">AVERAGE(H1:H114)</f>
+        <v>0.149000000000001</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C117" s="0" t="n">
+        <v>7.16804</v>
+      </c>
+      <c r="D117" s="0" t="n">
+        <v>1.576296</v>
+      </c>
+      <c r="G117" s="0" t="n">
+        <v>24.2187</v>
+      </c>
+      <c r="H117" s="0" t="n">
+        <v>29.2586</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C118" s="0" t="n">
+        <v>3.530937</v>
+      </c>
+      <c r="D118" s="0" t="n">
+        <v>4.957484</v>
+      </c>
+      <c r="G118" s="0" t="n">
+        <v>32.1591000000001</v>
+      </c>
+      <c r="H118" s="0" t="n">
+        <v>19.6083</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C119" s="0" t="n">
+        <v>4.902911</v>
+      </c>
+      <c r="D119" s="0" t="n">
+        <v>2.442658</v>
+      </c>
+      <c r="G119" s="0" t="n">
+        <v>15.3593999999999</v>
+      </c>
+      <c r="H119" s="0" t="n">
+        <v>10.9740999999999</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C120" s="0" t="n">
+        <v>3.981095</v>
+      </c>
+      <c r="D120" s="0" t="n">
+        <v>4.814818</v>
+      </c>
+      <c r="G120" s="0" t="n">
+        <v>14.2048</v>
+      </c>
+      <c r="H120" s="0" t="n">
+        <v>4.81850000000009</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C121" s="0" t="n">
+        <v>3.0398</v>
+      </c>
+      <c r="D121" s="0" t="n">
+        <v>3.414459</v>
+      </c>
+      <c r="G121" s="0" t="n">
+        <v>5.65300000000002</v>
+      </c>
+      <c r="H121" s="0" t="n">
+        <v>26.3071</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C122" s="0" t="n">
+        <v>3.313373</v>
+      </c>
+      <c r="D122" s="0" t="n">
+        <v>1.721964</v>
+      </c>
+      <c r="G122" s="0" t="n">
+        <v>10.9546</v>
+      </c>
+      <c r="H122" s="0" t="n">
+        <v>11.5749999999999</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C123" s="0" t="n">
+        <v>3.814527</v>
+      </c>
+      <c r="D123" s="0" t="n">
+        <v>4.145202</v>
+      </c>
+      <c r="G123" s="0" t="n">
+        <v>5.2509</v>
+      </c>
+      <c r="H123" s="0" t="n">
+        <v>2.00470000000007</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C124" s="0" t="n">
+        <v>3.435683</v>
+      </c>
+      <c r="D124" s="0" t="n">
+        <v>2.26528</v>
+      </c>
+      <c r="G124" s="0" t="n">
+        <v>5.7527</v>
+      </c>
+      <c r="H124" s="0" t="n">
+        <v>2.25839999999994</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C125" s="0" t="n">
+        <v>6.090559</v>
+      </c>
+      <c r="D125" s="0" t="n">
+        <v>4.300107</v>
+      </c>
+      <c r="G125" s="0" t="n">
+        <v>17.322</v>
+      </c>
+      <c r="H125" s="0" t="n">
+        <v>6.26430000000005</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B140" s="0" t="n">
+        <f aca="false">AVERAGE(B1:B136)</f>
+        <v>6.41888831578948</v>
+      </c>
+      <c r="C140" s="0" t="n">
+        <f aca="false">AVERAGE(C1:C136)</f>
+        <v>4.52884183902439</v>
+      </c>
+      <c r="D140" s="0" t="n">
+        <f aca="false">AVERAGE(D1:D136)</f>
+        <v>3.5917053664</v>
+      </c>
+      <c r="E140" s="0" t="n">
+        <f aca="false">AVERAGE(E1:E136)</f>
         <v>2.55301578133333</v>
       </c>
-      <c r="I116" s="0" t="n">
-        <f aca="false">AVERAGE(I1:I114)</f>
-        <v>11.9854278666667</v>
-      </c>
-    </row>
-    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="0" t="s">
+      <c r="F140" s="0" t="n">
+        <f aca="false">AVERAGE(F1:F136)</f>
+        <v>17.8150831578947</v>
+      </c>
+      <c r="G140" s="0" t="n">
+        <f aca="false">AVERAGE(G1:G136)</f>
+        <v>12.7318647073171</v>
+      </c>
+      <c r="H140" s="0" t="n">
+        <f aca="false">AVERAGE(H1:H136)</f>
+        <v>13.75078888</v>
+      </c>
+      <c r="I140" s="0" t="n">
+        <f aca="false">AVERAGE(I1:I136)</f>
+        <v>11.8194372</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="B117" s="0" t="n">
-        <f aca="false">STDEV(B1:B114)</f>
-        <v>3.60920890006673</v>
-      </c>
-      <c r="C117" s="0" t="n">
-        <f aca="false">STDEV(C1:C114)</f>
-        <v>27.4178337928726</v>
-      </c>
-      <c r="D117" s="0" t="n">
-        <f aca="false">STDEV(D1:D114)</f>
-        <v>2.5675416215042</v>
-      </c>
-      <c r="E117" s="0" t="n">
-        <f aca="false">STDEV(E1:E114)</f>
-        <v>12.6950325332175</v>
-      </c>
-      <c r="F117" s="0" t="n">
-        <f aca="false">STDEV(F1:F114)</f>
-        <v>1.60803532172332</v>
-      </c>
-      <c r="G117" s="0" t="n">
-        <f aca="false">STDEV(G1:G114)</f>
-        <v>24.6168597016759</v>
-      </c>
-      <c r="H117" s="0" t="n">
-        <f aca="false">STDEV(H1:H114)</f>
+      <c r="B141" s="0" t="n">
+        <f aca="false">STDEV(B1:B136)</f>
+        <v>3.60464938019423</v>
+      </c>
+      <c r="C141" s="0" t="n">
+        <f aca="false">STDEV(C1:C136)</f>
+        <v>2.50405569082915</v>
+      </c>
+      <c r="D141" s="0" t="n">
+        <f aca="false">STDEV(D1:D136)</f>
+        <v>1.59056711575682</v>
+      </c>
+      <c r="E141" s="0" t="n">
+        <f aca="false">STDEV(E1:E136)</f>
         <v>1.33466724369686</v>
       </c>
-      <c r="I117" s="0" t="n">
-        <f aca="false">STDEV(I1:I114)</f>
-        <v>11.6760984583963</v>
-      </c>
-    </row>
-    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B119" s="0" t="n">
+      <c r="F141" s="0" t="n">
+        <f aca="false">STDEV(F1:F136)</f>
+        <v>18.2878914383997</v>
+      </c>
+      <c r="G141" s="0" t="n">
+        <f aca="false">STDEV(G1:G136)</f>
+        <v>9.66642366205755</v>
+      </c>
+      <c r="H141" s="0" t="n">
+        <f aca="false">STDEV(H1:H136)</f>
+        <v>13.4935243912595</v>
+      </c>
+      <c r="I141" s="0" t="n">
+        <f aca="false">STDEV(I1:I136)</f>
+        <v>11.591888720145</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B143" s="0" t="n">
         <f aca="false">AVERAGE(B1:B2,B20:B21,B39:B40,B58:B59,B77:B78)</f>
         <v>3.7783024</v>
       </c>
-      <c r="C119" s="0" t="n">
-        <f aca="false">AVERAGE(D1:D2,D20:D21,D39:D40,D58:D59,D77:D78,D96:D97)</f>
-        <v>3.4476887</v>
-      </c>
-      <c r="D119" s="0" t="n">
-        <f aca="false">AVERAGE(F1:F2,F20:F21,F39:F40,F58:F59,F77:F78,F96:F97)</f>
-        <v>1.88981958333333</v>
-      </c>
-      <c r="E119" s="0" t="n">
-        <f aca="false">AVERAGE(H1:H2,H20:H21,H39:H40,H58:H59,H77:H78)</f>
+      <c r="C143" s="0" t="n">
+        <f aca="false">AVERAGE(C1:C2,C20:C21,C39:C40,C58:C59,C77:C78,C96:C97,C115:C116)</f>
+        <v>3.23156291666667</v>
+      </c>
+      <c r="D143" s="0" t="n">
+        <f aca="false">AVERAGE(D1:D2,D20:D21,D39:D40,D58:D59,D77:D78,D96:D97,D115:D116)</f>
+        <v>1.9941035</v>
+      </c>
+      <c r="E143" s="0" t="n">
+        <f aca="false">AVERAGE(E1:E2,E20:E21,E39:E40,E58:E59)</f>
         <v>1.98521314285714</v>
       </c>
-      <c r="F119" s="0" t="n">
-        <f aca="false">AVERAGE(C1:C2,C20:C21,C39:C40,C58:C59,C77:C78)</f>
+      <c r="F143" s="0" t="n">
+        <f aca="false">AVERAGE(F1:F2,F20:F21,F39:F40,F58:F59,F77:F78)</f>
         <v>25.94554</v>
       </c>
-      <c r="G119" s="0" t="n">
-        <f aca="false">AVERAGE(E1:E2,E20:E21,E39:E40,E58:E59,E77:E78,E96:E97)</f>
-        <v>14.1987279</v>
-      </c>
-      <c r="H119" s="0" t="n">
-        <f aca="false">AVERAGE(G1:G2,G20:G21,G39:G40,G58:G59,G77:G78,G96:G97)</f>
-        <v>14.5109091666667</v>
-      </c>
-      <c r="I119" s="0" t="n">
-        <f aca="false">AVERAGE(I1:I2,I20:I21,I39:I40,I58:I59,I77:I78)</f>
+      <c r="G143" s="0" t="n">
+        <f aca="false">AVERAGE(G1:G2,G20:G21,G39:G40,G58:G59,G77:G78,G96:G97,G115:G116)</f>
+        <v>15.1208649166667</v>
+      </c>
+      <c r="H143" s="0" t="n">
+        <f aca="false">AVERAGE(H1:H2,H20:H21,H39:H40,H58:H59,H77:H78,H96:H97,H115:H116)</f>
+        <v>15.3844792857143</v>
+      </c>
+      <c r="I143" s="0" t="n">
+        <f aca="false">AVERAGE(I1:I2,I20:I21,I39:I40,I58:I59)</f>
         <v>18.8979042857143</v>
       </c>
-    </row>
-    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B120" s="0" t="n">
+      <c r="L143" s="0" t="n">
+        <f aca="false">TTEST(B143:B146,C143:C146,1,2)</f>
+        <v>0.134090091555482</v>
+      </c>
+      <c r="M143" s="0" t="n">
+        <f aca="false">TTEST(B143:B146,D143:D146,1,2)</f>
+        <v>0.0270228770025976</v>
+      </c>
+      <c r="N143" s="0" t="n">
+        <f aca="false">TTEST(B143:B146,E143:E146,1,2)</f>
+        <v>0.0150301997534111</v>
+      </c>
+      <c r="O143" s="0" t="n">
+        <f aca="false">TTEST(F143:F146,G143:G146,1,2)</f>
+        <v>0.0811197475388893</v>
+      </c>
+      <c r="P143" s="0" t="n">
+        <f aca="false">TTEST(F143:F146,H143:H146,1,2)</f>
+        <v>0.159103399589221</v>
+      </c>
+      <c r="Q143" s="0" t="n">
+        <f aca="false">TTEST(F143:F146,I143:I146,1,2)</f>
+        <v>0.0765058319613057</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B144" s="0" t="n">
         <f aca="false">AVERAGE(B3,B22,B41,B60,B79)</f>
         <v>10.0790716</v>
       </c>
-      <c r="C120" s="0" t="n">
-        <f aca="false">AVERAGE(D3,D22,D41,D60,D79,D98)</f>
-        <v>7.175025</v>
-      </c>
-      <c r="D120" s="0" t="n">
-        <f aca="false">AVERAGE(F3,F22,F41,F60,F79,F98)</f>
-        <v>4.532124</v>
-      </c>
-      <c r="E120" s="0" t="n">
-        <f aca="false">AVERAGE(H3,H22,H41,H60,H79)</f>
+      <c r="C144" s="0" t="n">
+        <f aca="false">AVERAGE(C3,C22,C41,C60,C79,C98,C117)</f>
+        <v>7.17402714285714</v>
+      </c>
+      <c r="D144" s="0" t="n">
+        <f aca="false">AVERAGE(D3,D22,D41,D60,D79,D98,D117)</f>
+        <v>4.10986285714286</v>
+      </c>
+      <c r="E144" s="0" t="n">
+        <f aca="false">AVERAGE(E3,E22,E41,E60)</f>
         <v>4.2182385</v>
       </c>
-      <c r="F120" s="0" t="n">
-        <f aca="false">AVERAGE(C3,C22,C41,C60,C79)</f>
+      <c r="F144" s="0" t="n">
+        <f aca="false">AVERAGE(F3,F22,F41,F60,F79)</f>
         <v>35.081</v>
       </c>
-      <c r="G120" s="0" t="n">
-        <f aca="false">AVERAGE(E3,E22,E41,E60,E79,E98)</f>
+      <c r="G144" s="0" t="n">
+        <f aca="false">AVERAGE(G3,G22,G41,G60,G79,G98)</f>
         <v>20.80139</v>
       </c>
-      <c r="H120" s="0" t="n">
-        <f aca="false">AVERAGE(G3,G22,G41,G60,G79,G98)</f>
-        <v>26.2237666666667</v>
-      </c>
-      <c r="I120" s="0" t="n">
-        <f aca="false">AVERAGE(I3,I22,I41,I60,I79)</f>
+      <c r="H144" s="0" t="n">
+        <f aca="false">AVERAGE(H3,H22,H41,H60,H79,H98,H117)</f>
+        <v>26.6573142857143</v>
+      </c>
+      <c r="I144" s="0" t="n">
+        <f aca="false">AVERAGE(I3,I22,I41,I60)</f>
         <v>17.8213374999999</v>
       </c>
-    </row>
-    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="0" t="s">
+      <c r="L144" s="0" t="n">
+        <f aca="false">TTEST(C143:C146,D143:D146,1,2)</f>
+        <v>0.0948381602462979</v>
+      </c>
+      <c r="M144" s="0" t="n">
+        <f aca="false">TTEST(C143:C146,E143:E146,1,2)</f>
+        <v>0.0398781966153526</v>
+      </c>
+      <c r="O144" s="0" t="n">
+        <f aca="false">TTEST(G143:G146,H143:H146,1,2)</f>
+        <v>0.330849869456314</v>
+      </c>
+      <c r="P144" s="0" t="n">
+        <f aca="false">TTEST(G143:G146,I143:I146,1,2)</f>
+        <v>0.453638582635555</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="B121" s="0" t="n">
+      <c r="B145" s="0" t="n">
         <f aca="false">AVERAGE(B4:B11,B23:B30,B42:B49,B61:B68,B80:B87)</f>
-        <v>6.563674825</v>
-      </c>
-      <c r="C121" s="0" t="n">
-        <f aca="false">AVERAGE(D4:D11,D23:D30,D42:D49,D61:D68,D80:D87)</f>
-        <v>4.649203065</v>
-      </c>
-      <c r="D121" s="0" t="n">
+        <v>6.7990817</v>
+      </c>
+      <c r="C145" s="0" t="n">
+        <f aca="false">AVERAGE(C4:C11,C23:C30,C42:C49,C61:C68,C80:C87,C118:C125)</f>
+        <v>4.65840011666667</v>
+      </c>
+      <c r="D145" s="0" t="n">
+        <f aca="false">AVERAGE(D4:D11,D23:D30,D42:D49,D61:D68,D80:D87,D99:D106,D118:D125)</f>
+        <v>3.64409467678571</v>
+      </c>
+      <c r="E145" s="0" t="n">
+        <f aca="false">AVERAGE(E4:E11,E23:E30,E42:E49,E61:E68)</f>
+        <v>2.631863059375</v>
+      </c>
+      <c r="F145" s="0" t="n">
         <f aca="false">AVERAGE(F4:F11,F23:F30,F42:F49,F61:F68,F80:F87)</f>
-        <v>3.3865851725</v>
-      </c>
-      <c r="E121" s="0" t="n">
-        <f aca="false">AVERAGE(H4:H11,H23:H30,H42:H49,H61:H68,H80:H87)</f>
-        <v>2.631863059375</v>
-      </c>
-      <c r="F121" s="0" t="n">
-        <f aca="false">AVERAGE(C4:C11,C23:C30,C42:C49,C61:C68,C80:C87)</f>
-        <v>21.5835025</v>
-      </c>
-      <c r="G121" s="0" t="n">
-        <f aca="false">AVERAGE(E4:E11,E23:E30,E42:E49,E61:E68,E80:E87)</f>
-        <v>14.5015625</v>
-      </c>
-      <c r="H121" s="0" t="n">
-        <f aca="false">AVERAGE(G4:G11,G23:G30,G42:G49,G61:G68,G80:G87)</f>
-        <v>18.573855</v>
-      </c>
-      <c r="I121" s="0" t="n">
-        <f aca="false">AVERAGE(I4:I11,I23:I30,I42:I49,I61:I68,I80:I87)</f>
+        <v>17.205985</v>
+      </c>
+      <c r="G145" s="0" t="n">
+        <f aca="false">AVERAGE(G4:G11,G23:G30,G42:G49,G61:G68,G80:G87,G99:G106,G118:G125)</f>
+        <v>12.3622875</v>
+      </c>
+      <c r="H145" s="0" t="n">
+        <f aca="false">AVERAGE(H4:H11,H23:H30,H42:H49,H61:H68,H80:H87,H99:H106,H118:H125)</f>
+        <v>14.4485107142857</v>
+      </c>
+      <c r="I145" s="0" t="n">
+        <f aca="false">AVERAGE(I4:I11,I23:I30,I42:I49,I61:I68)</f>
         <v>12.5573125</v>
       </c>
-    </row>
-    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="0" t="s">
+      <c r="L145" s="0" t="n">
+        <f aca="false">TTEST(D143:D146,E143:E146,1,2)</f>
+        <v>0.204414364336538</v>
+      </c>
+      <c r="O145" s="0" t="n">
+        <f aca="false">TTEST(H143:H146,I143:I146,1,2)</f>
+        <v>0.304942687547591</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="B122" s="0" t="n">
+      <c r="B146" s="0" t="n">
         <f aca="false">AVERAGE(B12:B19,B31:B38,B50:B57,B69:B76,B88:B95)</f>
-        <v>6.21585095</v>
-      </c>
-      <c r="C122" s="0" t="n">
-        <f aca="false">AVERAGE(D12:D19,D31:D38,D50:D57,D69:D76,D88:D95)</f>
-        <v>4.33922634</v>
-      </c>
-      <c r="D122" s="0" t="n">
+        <v>6.2413185</v>
+      </c>
+      <c r="C146" s="0" t="n">
+        <f aca="false">AVERAGE(C12:C19,C31:C38,C50:C57,C69:C76,C88:C95,C107:C114)</f>
+        <v>4.30935628333333</v>
+      </c>
+      <c r="D146" s="0" t="n">
+        <f aca="false">AVERAGE(D12:D19,D31:D38,D50:D57,D69:D76,D88:D95,D107:D114)</f>
+        <v>3.92098708125</v>
+      </c>
+      <c r="E146" s="0" t="n">
+        <f aca="false">AVERAGE(E12:E19,E31:E38,E50:E57,E69:E76)</f>
+        <v>2.390222490625</v>
+      </c>
+      <c r="F146" s="0" t="n">
         <f aca="false">AVERAGE(F12:F19,F31:F38,F50:F57,F69:F76,F88:F95)</f>
-        <v>3.7169370225</v>
-      </c>
-      <c r="E122" s="0" t="n">
-        <f aca="false">AVERAGE(H12:H19,H31:H38,H50:H57,H69:H76,H88:H95)</f>
-        <v>2.390222490625</v>
-      </c>
-      <c r="F122" s="0" t="n">
-        <f aca="false">AVERAGE(C12:C19,C31:C38,C50:C57,C69:C76,C88:C95)</f>
-        <v>15.4955525</v>
-      </c>
-      <c r="G122" s="0" t="n">
-        <f aca="false">AVERAGE(E12:E19,E31:E38,E50:E57,E69:E76,E88:E95)</f>
-        <v>11.283486</v>
-      </c>
-      <c r="H122" s="0" t="n">
-        <f aca="false">AVERAGE(G12:G19,G31:G38,G50:G57,G69:G76,G88:G95)</f>
-        <v>13.62495</v>
-      </c>
-      <c r="I122" s="0" t="n">
-        <f aca="false">AVERAGE(I12:I19,I31:I38,I50:I57,I69:I76,I88:I95)</f>
-        <v>9.1719503125</v>
-      </c>
-    </row>
-    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="0" t="s">
+        <v>14.2333275</v>
+      </c>
+      <c r="G146" s="0" t="n">
+        <f aca="false">AVERAGE(G12:G19,G31:G38,G50:G57,G69:G76,G88:G95,G107:G114)</f>
+        <v>11.3177883333333</v>
+      </c>
+      <c r="H146" s="0" t="n">
+        <f aca="false">AVERAGE(H12:H19,H31:H38,H50:H57,H69:H76,H88:H95,H107:H114)</f>
+        <v>10.5780854166667</v>
+      </c>
+      <c r="I146" s="0" t="n">
+        <f aca="false">AVERAGE(I12:I19,I31:I38,I50:I57,I69:I76)</f>
+        <v>8.7829096875</v>
+      </c>
+    </row>
+    <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="B124" s="2" t="n">
+      <c r="B148" s="2" t="n">
         <f aca="false">STDEV(B1:B2,B20:B21,B39:B40,B58:B59,B77:B78)</f>
         <v>1.67706871606438</v>
       </c>
-      <c r="C124" s="2" t="n">
+      <c r="C148" s="2" t="n">
+        <f aca="false">STDEV(C1:C2,C20:C21,C39:C40,C58:C59,C77:C78,C96:C97)</f>
+        <v>2.96169461514211</v>
+      </c>
+      <c r="D148" s="2" t="n">
         <f aca="false">STDEV(D1:D2,D20:D21,D39:D40,D58:D59,D77:D78,D96:D97)</f>
-        <v>2.96169461514211</v>
-      </c>
-      <c r="D124" s="2" t="n">
-        <f aca="false">STDEV(F1:F2,F20:F21,F39:F40,F58:F59,F77:F78,F96:F97)</f>
         <v>0.87180451993932</v>
       </c>
-      <c r="E124" s="2" t="n">
-        <f aca="false">STDEV(H1:H2,H20:H21,H39:H40,H58:H59,H77:H78)</f>
+      <c r="E148" s="2" t="n">
+        <f aca="false">STDEV(E1:E2,E20:E21,E39:E40,E58:E59,E77:E78)</f>
         <v>0.838332004991346</v>
       </c>
-      <c r="F124" s="2" t="n">
-        <f aca="false">STDEV(C1:C2,C20:C21,C39:C40,C58:C59,C77:C78)</f>
+      <c r="F148" s="2" t="n">
+        <f aca="false">STDEV(F1:F2,F20:F21,F39:F40,F58:F59,F77:F78)</f>
         <v>30.8975171779654</v>
       </c>
-      <c r="G124" s="2" t="n">
-        <f aca="false">STDEV(E1:E2,E20:E21,E39:E40,E58:E59,E77:E78,E96:E97)</f>
-        <v>18.4611009883422</v>
-      </c>
-      <c r="H124" s="2" t="n">
-        <f aca="false">STDEV(G1:G2,G20:G21,G39:G40,G58:G59,G77:G78,G96:G97)</f>
-        <v>16.6728538174382</v>
-      </c>
-      <c r="I124" s="2" t="n">
+      <c r="G148" s="2" t="n">
+        <f aca="false">STDEV(G1:G2,G20:G21,G39:G40,G58:G59,G77:G78,G96:G97,G115:G116)</f>
+        <v>17.3349183234601</v>
+      </c>
+      <c r="H148" s="2" t="n">
+        <f aca="false">STDEV(H1:H2,H20:H21,H39:H40,H58:H59,H77:H78,H96:H97,H115:H116)</f>
+        <v>17.4544108268397</v>
+      </c>
+      <c r="I148" s="2" t="n">
         <f aca="false">STDEV(I1:I2,I20:I21,I39:I40,I58:I59,I77:I78)</f>
         <v>19.8192797988817</v>
       </c>
     </row>
-    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="0" t="s">
+    <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B125" s="2" t="n">
+      <c r="B149" s="2" t="n">
         <f aca="false">STDEV(B3,B22,B41,B60,B79)</f>
         <v>3.97531812653582</v>
       </c>
-      <c r="C125" s="2" t="n">
-        <f aca="false">STDEV(D3,D22,D41,D60,D79,D98)</f>
+      <c r="C149" s="2" t="n">
+        <f aca="false">STDEV(C3,C22,C41,C60,C79,C98)</f>
         <v>3.08407242584632</v>
       </c>
-      <c r="D125" s="2" t="n">
-        <f aca="false">STDEV(F3,F22,F41,F60,F79,F98)</f>
-        <v>2.18615794864141</v>
-      </c>
-      <c r="E125" s="2" t="n">
-        <f aca="false">STDEV(H3,H22,H41,H60,H79)</f>
+      <c r="D149" s="2" t="n">
+        <f aca="false">STDEV(D3,D22,D41,D60,D79,D98,D117)</f>
+        <v>2.28710955641449</v>
+      </c>
+      <c r="E149" s="2" t="n">
+        <f aca="false">STDEV(E3,E22,E41,E60,E79)</f>
         <v>1.420891915883</v>
       </c>
-      <c r="F125" s="2" t="n">
-        <f aca="false">STDEV(C3,C22,C41,C60,C79)</f>
+      <c r="F149" s="2" t="n">
+        <f aca="false">STDEV(F3,F22,F41,F60,F79)</f>
         <v>12.1181700943253</v>
       </c>
-      <c r="G125" s="2" t="n">
-        <f aca="false">STDEV(E3,E22,E41,E60,E79,E98)</f>
-        <v>7.50166590638373</v>
-      </c>
-      <c r="H125" s="2" t="n">
-        <f aca="false">STDEV(G3,G22,G41,G60,G79,G98)</f>
-        <v>13.0491007257461</v>
-      </c>
-      <c r="I125" s="2" t="n">
+      <c r="G149" s="2" t="n">
+        <f aca="false">STDEV(G3,G22,G41,G60,G79,G98,G117)</f>
+        <v>6.96879565977201</v>
+      </c>
+      <c r="H149" s="2" t="n">
+        <f aca="false">STDEV(H3,H22,H41,H60,H79,H98,H117)</f>
+        <v>11.9672443037134</v>
+      </c>
+      <c r="I149" s="2" t="n">
         <f aca="false">STDEV(I3,I22,I41,I60,I79)</f>
         <v>4.63392682099008</v>
       </c>
     </row>
-    <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="0" t="s">
+    <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="B126" s="2" t="n">
+      <c r="B150" s="2" t="n">
         <f aca="false">STDEV(B4:B11,B23:B30,B42:B49,B61:B68,B80:B87)</f>
-        <v>3.65248433761856</v>
-      </c>
-      <c r="C126" s="2" t="n">
-        <f aca="false">STDEV(D4:D11,D23:D30,D42:D49,D61:D68,D80:D87,D99:D106)</f>
-        <v>2.16893288554737</v>
-      </c>
-      <c r="D126" s="2" t="n">
-        <f aca="false">STDEV(F4:F11,F23:F30,F42:F49,F61:F68,F80:F87,F99:F106)</f>
-        <v>1.49827617723526</v>
-      </c>
-      <c r="E126" s="2" t="n">
-        <f aca="false">STDEV(H4:H11,H23:H30,H42:H49,H61:H68,H80:H87)</f>
+        <v>3.6249482812041</v>
+      </c>
+      <c r="C150" s="2" t="n">
+        <f aca="false">STDEV(C4:C11,C23:C30,C42:C49,C61:C68,C80:C87,C99:C106,C118:C125)</f>
+        <v>2.06550634334098</v>
+      </c>
+      <c r="D150" s="2" t="n">
+        <f aca="false">STDEV(D4:D11,D23:D30,D42:D49,D61:D68,D80:D87,D99:D106,D118:D125)</f>
+        <v>1.45964612618933</v>
+      </c>
+      <c r="E150" s="2" t="n">
+        <f aca="false">STDEV(E4:E11,E23:E30,E42:E49,E61:E68,E80:E87)</f>
         <v>1.38459709223569</v>
       </c>
-      <c r="F126" s="2" t="n">
-        <f aca="false">STDEV(C4:C11,C23:C30,C42:C49,C61:C68,C80:C87)</f>
-        <v>34.0506090626087</v>
-      </c>
-      <c r="G126" s="2" t="n">
-        <f aca="false">STDEV(E4:E11,E23:E30,E42:E49,E61:E68,E80:E87,E99:E106)</f>
-        <v>14.9159982833363</v>
-      </c>
-      <c r="H126" s="2" t="n">
+      <c r="F150" s="2" t="n">
+        <f aca="false">STDEV(F4:F11,F23:F30,F42:F49,F61:F68,F80:F87)</f>
+        <v>17.0065867829173</v>
+      </c>
+      <c r="G150" s="2" t="n">
         <f aca="false">STDEV(G4:G11,G23:G30,G42:G49,G61:G68,G80:G87,G99:G106)</f>
-        <v>27.4091726422981</v>
-      </c>
-      <c r="I126" s="2" t="n">
-        <f aca="false">STDEV(I4:I11,I23:I30,I42:I49,I61:I68,I80:I87)</f>
+        <v>8.02967697468592</v>
+      </c>
+      <c r="H150" s="2" t="n">
+        <f aca="false">STDEV(H4:H11,H23:H30,H42:H49,H61:H68,H80:H87,H99:H106)</f>
+        <v>15.0218740460329</v>
+      </c>
+      <c r="I150" s="2" t="n">
+        <f aca="false">STDEV(I4:I11,I23:I30,I42:I49,I61:I68)</f>
         <v>12.2278251765218</v>
       </c>
     </row>
-    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="0" t="s">
+    <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B127" s="2" t="n">
+      <c r="B151" s="2" t="n">
         <f aca="false">STDEV(B12:B19,B31:B38,B50:B57,B69:B76,B88:B95)</f>
-        <v>3.49951252399826</v>
-      </c>
-      <c r="C127" s="2" t="n">
+        <v>3.49592641559815</v>
+      </c>
+      <c r="C151" s="2" t="n">
+        <f aca="false">STDEV(C12:C19,C31:C38,C50:C57,C69:C76,C88:C95,C107:C114)</f>
+        <v>2.63903759172088</v>
+      </c>
+      <c r="D151" s="2" t="n">
         <f aca="false">STDEV(D12:D19,D31:D38,D50:D57,D69:D76,D88:D95,D107:D114)</f>
-        <v>2.63903759172088</v>
-      </c>
-      <c r="D127" s="2" t="n">
-        <f aca="false">STDEV(F12:F19,F31:F38,F50:F57,F69:F76,F88:F95,F107:F114)</f>
-        <v>1.53568217035489</v>
-      </c>
-      <c r="E127" s="2" t="n">
-        <f aca="false">STDEV(H12:H19,H31:H38,H50:H57,H69:H76,H88:H95)</f>
+        <v>1.54980398236121</v>
+      </c>
+      <c r="E151" s="2" t="n">
+        <f aca="false">STDEV(E12:E19,E31:E38,E50:E57,E69:E76,E88:E95)</f>
         <v>1.24069785022728</v>
       </c>
-      <c r="F127" s="2" t="n">
-        <f aca="false">STDEV(C12:C19,C31:C38,C50:C57,C69:C76,C88:C95)</f>
-        <v>18.856102626797</v>
-      </c>
-      <c r="G127" s="2" t="n">
-        <f aca="false">STDEV(E12:E19,E31:E38,E50:E57,E69:E76,E88:E95,E107:E114)</f>
+      <c r="F151" s="2" t="n">
+        <f aca="false">STDEV(F12:F19,F31:F38,F50:F57,F69:F76,F88:F95)</f>
+        <v>14.5878143315856</v>
+      </c>
+      <c r="G151" s="2" t="n">
+        <f aca="false">STDEV(G12:G19,G31:G38,G50:G57,G69:G76,G88:G95,G107:G114)</f>
         <v>8.64950463913798</v>
       </c>
-      <c r="H127" s="2" t="n">
-        <f aca="false">STDEV(G12:G19,G31:G38,G50:G57,G69:G76,G88:G95,G107:G114)</f>
-        <v>24.4185268620325</v>
-      </c>
-      <c r="I127" s="2" t="n">
-        <f aca="false">STDEV(I12:I19,I31:I38,I50:I57,I69:I76,I88:I95)</f>
-        <v>8.60923383620224</v>
-      </c>
-    </row>
-    <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="H151" s="2" t="n">
+        <f aca="false">STDEV(H12:H19,H31:H38,H50:H57,H69:H76,H88:H95,H107:H114)</f>
+        <v>10.0699771906604</v>
+      </c>
+      <c r="I151" s="2" t="n">
+        <f aca="false">STDEV(I12:I19,I31:I38,I50:I57,I69:I76)</f>
+        <v>8.1909917364546</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B155" s="0" t="n">
+        <f aca="false">AVERAGE(B143:B146)</f>
+        <v>6.72444355</v>
+      </c>
+      <c r="C155" s="0" t="n">
+        <f aca="false">AVERAGE(C143:C146)</f>
+        <v>4.84333661488095</v>
+      </c>
+      <c r="D155" s="0" t="n">
+        <f aca="false">AVERAGE(D143:D146)</f>
+        <v>3.41726202879464</v>
+      </c>
+      <c r="E155" s="0" t="n">
+        <f aca="false">AVERAGE(E143:E146)</f>
+        <v>2.80638429821429</v>
+      </c>
+      <c r="F155" s="0" t="n">
+        <f aca="false">AVERAGE(F143:F146)</f>
+        <v>23.116463125</v>
+      </c>
+      <c r="G155" s="0" t="n">
+        <f aca="false">AVERAGE(G143:G146)</f>
+        <v>14.9005826875</v>
+      </c>
+      <c r="H155" s="0" t="n">
+        <f aca="false">AVERAGE(H143:H146)</f>
+        <v>16.7670974255952</v>
+      </c>
+      <c r="I155" s="0" t="n">
+        <f aca="false">AVERAGE(I143:I146)</f>
+        <v>14.5148659933035</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L156" s="0" t="n">
+        <v>6.41888831578948</v>
+      </c>
+      <c r="M156" s="0" t="n">
+        <v>4.52884183902439</v>
+      </c>
+      <c r="N156" s="0" t="n">
+        <v>3.5917053664</v>
+      </c>
+      <c r="O156" s="0" t="n">
+        <v>2.55301578133333</v>
+      </c>
+      <c r="P156" s="0" t="n">
+        <v>17.8150831578947</v>
+      </c>
+      <c r="Q156" s="0" t="n">
+        <v>12.7318647073171</v>
+      </c>
+      <c r="R156" s="0" t="n">
+        <v>13.75078888</v>
+      </c>
+      <c r="S156" s="0" t="n">
+        <v>11.8194372</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L157" s="0" t="n">
+        <v>3.60464938019423</v>
+      </c>
+      <c r="M157" s="0" t="n">
+        <v>2.50405569082915</v>
+      </c>
+      <c r="N157" s="0" t="n">
+        <v>1.59056711575682</v>
+      </c>
+      <c r="O157" s="0" t="n">
+        <v>1.33466724369686</v>
+      </c>
+      <c r="P157" s="0" t="n">
+        <v>18.2878914383997</v>
+      </c>
+      <c r="Q157" s="0" t="n">
+        <v>9.66642366205755</v>
+      </c>
+      <c r="R157" s="0" t="n">
+        <v>13.4935243912595</v>
+      </c>
+      <c r="S157" s="0" t="n">
+        <v>11.591888720145</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>